<commit_message>
Updated business model for Tourism. Updated effort in service for Brij from opt management to proj management
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="8" r:id="rId1"/>
@@ -24,12 +24,12 @@
     <definedName name="MemberList">'Team Member'!$B$4:$B$10</definedName>
     <definedName name="SkillList">'Skill Set'!$C$2:$C$34</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="88">
   <si>
     <t>Total</t>
   </si>
@@ -287,16 +287,22 @@
   </si>
   <si>
     <t>Discussion of project</t>
+  </si>
+  <si>
+    <t>23.10.2016</t>
+  </si>
+  <si>
+    <t>Updating business model to target April 2016 launch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1109,6 +1115,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1143,6 +1150,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1318,12 +1326,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="1"/>
@@ -1331,8 +1339,8 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:15">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="19"/>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -1348,7 +1356,7 @@
       <c r="N2" s="20"/>
       <c r="O2" s="21"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1364,7 +1372,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="22"/>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1380,7 +1388,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="22"/>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1396,7 +1404,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="22"/>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1412,7 +1420,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="22"/>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1428,7 +1436,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="22"/>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1444,7 +1452,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="22"/>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1460,7 +1468,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="22"/>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1478,7 +1486,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="22"/>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1489,7 +1497,7 @@
       <c r="G11" s="78"/>
       <c r="H11" s="82">
         <f>Summery!D10</f>
-        <v>9232.985999999999</v>
+        <v>9304.0059999999994</v>
       </c>
       <c r="I11" s="83"/>
       <c r="J11" s="84"/>
@@ -1499,7 +1507,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="22"/>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1510,7 +1518,7 @@
       <c r="G12" s="78"/>
       <c r="H12" s="79">
         <f>Summery!C10</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I12" s="80"/>
       <c r="J12" s="81"/>
@@ -1520,7 +1528,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="22"/>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1531,7 +1539,7 @@
       <c r="G13" s="78"/>
       <c r="H13" s="79">
         <f>H12/8</f>
-        <v>2.625</v>
+        <v>3</v>
       </c>
       <c r="I13" s="80"/>
       <c r="J13" s="81"/>
@@ -1541,7 +1549,7 @@
       <c r="N13" s="4"/>
       <c r="O13" s="22"/>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1557,7 +1565,7 @@
       <c r="N14" s="4"/>
       <c r="O14" s="22"/>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1573,7 +1581,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="22"/>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1589,7 +1597,7 @@
       <c r="N16" s="4"/>
       <c r="O16" s="22"/>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
@@ -1604,7 +1612,7 @@
       <c r="N17" s="4"/>
       <c r="O17" s="22"/>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1619,7 +1627,7 @@
       <c r="N18" s="4"/>
       <c r="O18" s="22"/>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1635,7 +1643,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="22"/>
     </row>
-    <row r="20" spans="2:15" ht="15.75" thickBot="1">
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1668,12 +1676,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
@@ -1695,7 +1703,7 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="85" t="s">
         <v>62</v>
@@ -1716,7 +1724,7 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="11" t="s">
         <v>6</v>
@@ -1749,18 +1757,18 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="15">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" s="34">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>4734.8499999999995</v>
+        <v>6510.4299999999994</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
@@ -1784,7 +1792,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="10" t="s">
         <v>10</v>
@@ -1795,7 +1803,7 @@
       </c>
       <c r="D4" s="34">
         <f>SUMIF(Business!B:B,B4,Business!I:I) + SUMIF(School!B:B,B4,School!I:I) + SUMIF(Service!B:B,B4,Service!I:I)+SUMIF(Retail!B:B,B4,Retail!I:I) + SUMIF(Tourism!B:B,B4,Tourism!I:I)</f>
-        <v>3314.4160000000002</v>
+        <v>1609.8560000000002</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="10" t="s">
@@ -1819,7 +1827,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
@@ -1842,7 +1850,7 @@
       </c>
       <c r="H5" s="34">
         <f>SUM(Service!I:I)</f>
-        <v>4261.3919999999998</v>
+        <v>2556.8319999999999</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="4"/>
@@ -1854,7 +1862,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="10" t="s">
         <v>11</v>
@@ -1889,7 +1897,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="10" t="s">
         <v>12</v>
@@ -1908,11 +1916,11 @@
       </c>
       <c r="G7" s="15">
         <f>SUM(Tourism!D:D)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H7" s="34">
         <f>SUM(Tourism!I:I)</f>
-        <v>0</v>
+        <v>1775.58</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="4"/>
@@ -1924,7 +1932,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="10" t="s">
         <v>13</v>
@@ -1943,11 +1951,11 @@
       </c>
       <c r="G8" s="16">
         <f>SUM(G3:G7)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H8" s="35">
         <f>SUM(H3:H7)</f>
-        <v>9232.9860000000008</v>
+        <v>9304.0060000000012</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -1959,7 +1967,7 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="10" t="s">
         <v>14</v>
@@ -1986,18 +1994,18 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="16">
         <f>SUM(C3:C9)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" s="35">
         <f>SUM(D3:D9)</f>
-        <v>9232.985999999999</v>
+        <v>9304.0059999999994</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2013,7 +2021,7 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="17"/>
@@ -2029,7 +2037,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="17"/>
@@ -2045,7 +2053,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="17"/>
@@ -2064,7 +2072,7 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="17"/>
@@ -2083,7 +2091,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="17"/>
@@ -2102,7 +2110,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="17"/>
@@ -2121,7 +2129,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="17"/>
@@ -2140,7 +2148,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="17"/>
@@ -2173,14 +2181,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="66" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="58" bestFit="1" customWidth="1"/>
@@ -2195,7 +2203,7 @@
     <col min="11" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>4</v>
       </c>
@@ -2227,7 +2235,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>51</v>
       </c>
@@ -2264,7 +2272,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="59"/>
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
@@ -2291,7 +2299,7 @@
       </c>
       <c r="J3" s="65"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
@@ -2318,7 +2326,7 @@
       </c>
       <c r="J4" s="65"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="59"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -2345,7 +2353,7 @@
       </c>
       <c r="J5" s="65"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="59"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -2387,14 +2395,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="66" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="58" bestFit="1" customWidth="1"/>
@@ -2409,7 +2417,7 @@
     <col min="11" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>4</v>
       </c>
@@ -2441,7 +2449,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="59">
         <v>42298</v>
       </c>
@@ -2476,7 +2484,7 @@
       </c>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="59">
         <v>42299</v>
       </c>
@@ -2511,7 +2519,7 @@
       </c>
       <c r="J3" s="65"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
@@ -2538,7 +2546,7 @@
       </c>
       <c r="J4" s="65"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="59"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -2565,7 +2573,7 @@
       </c>
       <c r="J5" s="65"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="59"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -2606,14 +2614,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="66" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="58" bestFit="1" customWidth="1"/>
@@ -2628,7 +2636,7 @@
     <col min="11" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>4</v>
       </c>
@@ -2660,7 +2668,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="59"/>
       <c r="B2" s="60" t="s">
         <v>8</v>
@@ -2691,7 +2699,7 @@
       </c>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="59"/>
       <c r="B3" s="60" t="s">
         <v>8</v>
@@ -2722,7 +2730,7 @@
       </c>
       <c r="J3" s="65"/>
     </row>
-    <row r="4" spans="1:10" ht="30">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>77</v>
       </c>
@@ -2759,7 +2767,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>77</v>
       </c>
@@ -2767,14 +2775,14 @@
         <v>10</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="61">
         <v>4</v>
       </c>
       <c r="E5" s="62">
         <f>IF(ISERROR(MATCH(C5,SkillList,0)),0,MATCH(C5,SkillList,0))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="62">
         <f>IF(ISERROR(MATCH(B5,MemberList,0)),0,MATCH(B5,MemberList,0))</f>
@@ -2782,21 +2790,21 @@
       </c>
       <c r="G5" s="63">
         <f>INDEX(CostPerHour,E5)</f>
-        <v>591.86</v>
+        <v>236.74</v>
       </c>
       <c r="H5" s="64">
         <f>IF(ISERROR(INDEX(Competency,F5,E5)), 0, INDEX(Competency,F5,E5))</f>
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="I5" s="63">
         <f t="shared" si="0"/>
-        <v>1893.9520000000002</v>
+        <v>189.39200000000002</v>
       </c>
       <c r="J5" s="65" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="59"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -2837,14 +2845,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="66" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="58" bestFit="1" customWidth="1"/>
@@ -2859,7 +2867,7 @@
     <col min="11" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>4</v>
       </c>
@@ -2891,7 +2899,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>77</v>
       </c>
@@ -2928,7 +2936,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>77</v>
       </c>
@@ -2965,7 +2973,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>77</v>
       </c>
@@ -3002,7 +3010,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="59"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -3029,7 +3037,7 @@
       </c>
       <c r="J5" s="65"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="59"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -3070,14 +3078,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="66" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="58" bestFit="1" customWidth="1"/>
@@ -3092,7 +3100,7 @@
     <col min="11" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>4</v>
       </c>
@@ -3124,34 +3132,44 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="59"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="61"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="61">
+        <v>3</v>
+      </c>
       <c r="E2" s="62">
         <f>IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F2" s="62">
         <f>IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="63">
         <f>INDEX(CostPerHour,E2)</f>
-        <v>1183.71</v>
+        <v>591.86</v>
       </c>
       <c r="H2" s="64">
         <f>IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="63">
         <f>D2*G2*H2</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="65"/>
-    </row>
-    <row r="3" spans="1:10">
+        <v>1775.58</v>
+      </c>
+      <c r="J2" s="65" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="59"/>
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
@@ -3178,7 +3196,7 @@
       </c>
       <c r="J3" s="65"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
@@ -3205,7 +3223,7 @@
       </c>
       <c r="J4" s="65"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="59"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -3232,7 +3250,7 @@
       </c>
       <c r="J5" s="65"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="59"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -3273,14 +3291,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -3293,7 +3311,7 @@
     <col min="30" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="92" t="s">
         <v>83</v>
       </c>
@@ -3334,7 +3352,7 @@
       <c r="AH1" s="90"/>
       <c r="AI1" s="91"/>
     </row>
-    <row r="2" spans="1:35" s="27" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:35" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="93"/>
       <c r="B2" s="93"/>
       <c r="C2" s="94" t="s">
@@ -3381,7 +3399,7 @@
       <c r="AH2" s="87"/>
       <c r="AI2" s="88"/>
     </row>
-    <row r="3" spans="1:35" ht="180">
+    <row r="3" spans="1:35" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
@@ -3488,7 +3506,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="24">
         <v>1</v>
       </c>
@@ -3595,7 +3613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
         <v>2</v>
       </c>
@@ -3702,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
         <v>3</v>
       </c>
@@ -3743,7 +3761,7 @@
       <c r="AH6" s="36"/>
       <c r="AI6" s="45"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>4</v>
       </c>
@@ -3784,7 +3802,7 @@
       <c r="AH7" s="36"/>
       <c r="AI7" s="45"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="24">
         <v>5</v>
       </c>
@@ -3825,7 +3843,7 @@
       <c r="AH8" s="36"/>
       <c r="AI8" s="45"/>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>6</v>
       </c>
@@ -3866,7 +3884,7 @@
       <c r="AH9" s="36"/>
       <c r="AI9" s="45"/>
     </row>
-    <row r="10" spans="1:35" ht="15.75" thickBot="1">
+    <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24">
         <v>7</v>
       </c>
@@ -3989,14 +4007,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -4006,7 +4024,7 @@
     <col min="7" max="7" width="13.140625" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>71</v>
       </c>
@@ -4029,7 +4047,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="100" t="s">
         <v>25</v>
       </c>
@@ -4056,7 +4074,7 @@
       </c>
       <c r="H2" s="74"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="101"/>
       <c r="B3" s="9">
         <v>2</v>
@@ -4081,7 +4099,7 @@
       </c>
       <c r="H3" s="74"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="101"/>
       <c r="B4" s="9">
         <v>3</v>
@@ -4106,7 +4124,7 @@
       </c>
       <c r="H4" s="74"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="101"/>
       <c r="B5" s="9">
         <v>4</v>
@@ -4131,7 +4149,7 @@
       </c>
       <c r="H5" s="74"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="101"/>
       <c r="B6" s="9">
         <v>5</v>
@@ -4156,7 +4174,7 @@
       </c>
       <c r="H6" s="74"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="102"/>
       <c r="B7" s="9">
         <v>6</v>
@@ -4181,7 +4199,7 @@
       </c>
       <c r="H7" s="74"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="100" t="s">
         <v>29</v>
       </c>
@@ -4207,7 +4225,7 @@
         <v>591.86</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="101"/>
       <c r="B9" s="9">
         <v>8</v>
@@ -4231,7 +4249,7 @@
         <v>236.74</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="101"/>
       <c r="B10" s="9">
         <v>9</v>
@@ -4255,7 +4273,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="101"/>
       <c r="B11" s="9">
         <v>10</v>
@@ -4279,7 +4297,7 @@
         <v>591.86</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="101"/>
       <c r="B12" s="9">
         <v>11</v>
@@ -4303,7 +4321,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="101"/>
       <c r="B13" s="9">
         <v>12</v>
@@ -4327,7 +4345,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="101"/>
       <c r="B14" s="9">
         <v>13</v>
@@ -4351,7 +4369,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="101"/>
       <c r="B15" s="9">
         <v>14</v>
@@ -4375,7 +4393,7 @@
         <v>295.93</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="101"/>
       <c r="B16" s="9">
         <v>15</v>
@@ -4399,7 +4417,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="100" t="s">
         <v>69</v>
       </c>
@@ -4425,7 +4443,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="101"/>
       <c r="B18" s="9">
         <v>17</v>
@@ -4449,7 +4467,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="101"/>
       <c r="B19" s="9">
         <v>18</v>
@@ -4473,7 +4491,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="101"/>
       <c r="B20" s="9">
         <v>19</v>
@@ -4497,7 +4515,7 @@
         <v>236.74</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="101"/>
       <c r="B21" s="9">
         <v>20</v>
@@ -4521,7 +4539,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="101"/>
       <c r="B22" s="9">
         <v>21</v>
@@ -4545,7 +4563,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="101"/>
       <c r="B23" s="9">
         <v>22</v>
@@ -4569,7 +4587,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="101"/>
       <c r="B24" s="9">
         <v>23</v>
@@ -4593,7 +4611,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="101"/>
       <c r="B25" s="9">
         <v>24</v>
@@ -4617,7 +4635,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="102"/>
       <c r="B26" s="9">
         <v>25</v>
@@ -4641,7 +4659,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="100" t="s">
         <v>70</v>
       </c>
@@ -4667,7 +4685,7 @@
         <v>295.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="101"/>
       <c r="B28" s="9">
         <v>27</v>
@@ -4691,7 +4709,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="101"/>
       <c r="B29" s="9">
         <v>28</v>
@@ -4715,7 +4733,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="102"/>
       <c r="B30" s="9">
         <v>29</v>
@@ -4739,7 +4757,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="100" t="s">
         <v>28</v>
       </c>
@@ -4765,7 +4783,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="101"/>
       <c r="B32" s="9">
         <v>31</v>
@@ -4789,7 +4807,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="101"/>
       <c r="B33" s="9">
         <v>32</v>
@@ -4813,7 +4831,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="101"/>
       <c r="B34" s="9">
         <v>33</v>

</xml_diff>

<commit_message>
Adding effort for 23.10.2015 on service and review
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="8" r:id="rId1"/>
@@ -24,12 +24,12 @@
     <definedName name="MemberList">'Team Member'!$B$4:$B$10</definedName>
     <definedName name="SkillList">'Skill Set'!$C$2:$C$34</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="93">
   <si>
     <t>Total</t>
   </si>
@@ -214,9 +214,6 @@
     <t>Man Days</t>
   </si>
   <si>
-    <t>Man Day</t>
-  </si>
-  <si>
     <t>Personel</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     <t>Tourism</t>
   </si>
   <si>
-    <t>Hr</t>
-  </si>
-  <si>
     <t>Effort Calculation</t>
   </si>
   <si>
@@ -293,16 +287,37 @@
   </si>
   <si>
     <t>Updating business model to target April 2016 launch</t>
+  </si>
+  <si>
+    <t>24.10.2015</t>
+  </si>
+  <si>
+    <t>Discussion on Ascent project.</t>
+  </si>
+  <si>
+    <t>23.10.2015</t>
+  </si>
+  <si>
+    <t>Discussion on path and review</t>
+  </si>
+  <si>
+    <t>Man Hr</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Cost Per Anum!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -765,7 +780,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1115,6 +1129,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1149,6 +1164,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1324,12 +1340,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:J11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="1"/>
@@ -1337,24 +1355,24 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:15">
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="21"/>
-    </row>
-    <row r="3" spans="2:15">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="20"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1368,9 +1386,9 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="22"/>
-    </row>
-    <row r="4" spans="2:15">
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1384,9 +1402,9 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="22"/>
-    </row>
-    <row r="5" spans="2:15">
+      <c r="O4" s="21"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1400,9 +1418,9 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="22"/>
-    </row>
-    <row r="6" spans="2:15">
+      <c r="O5" s="21"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1416,9 +1434,9 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="22"/>
-    </row>
-    <row r="7" spans="2:15">
+      <c r="O6" s="21"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1432,9 +1450,9 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="22"/>
-    </row>
-    <row r="8" spans="2:15">
+      <c r="O7" s="21"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1448,9 +1466,9 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
-      <c r="O8" s="22"/>
-    </row>
-    <row r="9" spans="2:15">
+      <c r="O8" s="21"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1464,90 +1482,90 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="22"/>
-    </row>
-    <row r="10" spans="2:15">
+      <c r="O9" s="21"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
+      <c r="F10" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="22"/>
-    </row>
-    <row r="11" spans="2:15">
+      <c r="O10" s="21"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="77" t="s">
+      <c r="F11" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="78"/>
-      <c r="H11" s="82">
+      <c r="G11" s="77"/>
+      <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>10014.238000000001</v>
-      </c>
-      <c r="I11" s="83"/>
-      <c r="J11" s="84"/>
+        <v>10724.463</v>
+      </c>
+      <c r="I11" s="82"/>
+      <c r="J11" s="83"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="22"/>
-    </row>
-    <row r="12" spans="2:15">
+      <c r="O11" s="21"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="G12" s="78"/>
-      <c r="H12" s="79">
+      <c r="F12" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="77"/>
+      <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>24</v>
-      </c>
-      <c r="I12" s="80"/>
-      <c r="J12" s="81"/>
+        <v>25.5</v>
+      </c>
+      <c r="I12" s="79"/>
+      <c r="J12" s="80"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="22"/>
-    </row>
-    <row r="13" spans="2:15">
+      <c r="O12" s="21"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="77" t="s">
+      <c r="F13" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="78"/>
-      <c r="H13" s="79">
+      <c r="G13" s="77"/>
+      <c r="H13" s="78">
         <f>H12/8</f>
-        <v>3</v>
-      </c>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81"/>
+        <v>3.1875</v>
+      </c>
+      <c r="I13" s="79"/>
+      <c r="J13" s="80"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="22"/>
-    </row>
-    <row r="14" spans="2:15">
+      <c r="O13" s="21"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1561,9 +1579,9 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="22"/>
-    </row>
-    <row r="15" spans="2:15">
+      <c r="O14" s="21"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1577,9 +1595,9 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="22"/>
-    </row>
-    <row r="16" spans="2:15">
+      <c r="O15" s="21"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1593,9 +1611,9 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
-      <c r="O16" s="22"/>
-    </row>
-    <row r="17" spans="2:15">
+      <c r="O16" s="21"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
@@ -1608,9 +1626,9 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="22"/>
-    </row>
-    <row r="18" spans="2:15">
+      <c r="O17" s="21"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1623,9 +1641,9 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
-      <c r="O18" s="22"/>
-    </row>
-    <row r="19" spans="2:15">
+      <c r="O18" s="21"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1639,9 +1657,9 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="22"/>
-    </row>
-    <row r="20" spans="2:15" ht="15.75" thickBot="1">
+      <c r="O19" s="21"/>
+    </row>
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1655,7 +1673,7 @@
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
-      <c r="O20" s="23"/>
+      <c r="O20" s="22"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -1674,21 +1692,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -1701,17 +1721,19 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="85" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
+      <c r="B1" s="84" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
       <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="F1" s="84" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
@@ -1722,27 +1744,25 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>67</v>
-      </c>
+      <c r="E2" s="8"/>
       <c r="F2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="8"/>
@@ -1755,30 +1775,30 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>13</v>
-      </c>
-      <c r="D3" s="34">
+        <v>14.5</v>
+      </c>
+      <c r="D3" s="33">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>6510.4299999999994</v>
+        <v>7220.6549999999997</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="14">
         <f>SUM(Business!D:D)</f>
-        <v>5</v>
-      </c>
-      <c r="H3" s="34">
+        <v>5.5</v>
+      </c>
+      <c r="H3" s="33">
         <f>SUM(Business!I:I)</f>
-        <v>1775.5500000000002</v>
+        <v>2367.4050000000002</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="4"/>
@@ -1790,28 +1810,28 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <f>SUMIF(Business!B:B,B4,Business!D:D) + SUMIF(School!B:B,B4,School!D:D) + SUMIF(Service!B:B,B4,Service!D:D)+SUMIF(Retail!B:B,B4,Retail!D:D) + SUMIF(Tourism!B:B,B4,Tourism!D:D)</f>
         <v>7</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="33">
         <f>SUMIF(Business!B:B,B4,Business!I:I) + SUMIF(School!B:B,B4,School!I:I) + SUMIF(Service!B:B,B4,Service!I:I)+SUMIF(Retail!B:B,B4,Retail!I:I) + SUMIF(Tourism!B:B,B4,Tourism!I:I)</f>
         <v>1609.8560000000002</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="15">
+        <v>62</v>
+      </c>
+      <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
         <v>4</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
         <v>1893.9520000000002</v>
       </c>
@@ -1825,30 +1845,30 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <f>SUMIF(Business!B:B,B5,Business!D:D) + SUMIF(School!B:B,B5,School!D:D) + SUMIF(Service!B:B,B5,Service!D:D)+SUMIF(Retail!B:B,B5,Retail!D:D) + SUMIF(Tourism!B:B,B5,Tourism!D:D)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="33">
         <f>SUMIF(Business!B:B,B5,Business!I:I) + SUMIF(School!B:B,B5,School!I:I) + SUMIF(Service!B:B,B5,Service!I:I)+SUMIF(Retail!B:B,B5,Retail!I:I) + SUMIF(Tourism!B:B,B5,Tourism!I:I)</f>
         <v>0</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="15">
+        <v>63</v>
+      </c>
+      <c r="G5" s="14">
         <f>SUM(Service!D:D)</f>
-        <v>8</v>
-      </c>
-      <c r="H5" s="34">
+        <v>9</v>
+      </c>
+      <c r="H5" s="33">
         <f>SUM(Service!I:I)</f>
-        <v>2556.8319999999999</v>
+        <v>2675.2019999999998</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="4"/>
@@ -1860,28 +1880,28 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <f>SUMIF(Business!B:B,B6,Business!D:D) + SUMIF(School!B:B,B6,School!D:D) + SUMIF(Service!B:B,B6,Service!D:D)+SUMIF(Retail!B:B,B6,Retail!D:D) + SUMIF(Tourism!B:B,B6,Tourism!D:D)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="33">
         <f>SUMIF(Business!B:B,B6,Business!I:I) + SUMIF(School!B:B,B6,School!I:I) + SUMIF(Service!B:B,B6,Service!I:I)+SUMIF(Retail!B:B,B6,Retail!I:I) + SUMIF(Tourism!B:B,B6,Tourism!I:I)</f>
         <v>0</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="15">
+        <v>64</v>
+      </c>
+      <c r="G6" s="14">
         <f>SUM(Retail!D:D)</f>
         <v>4</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="33">
         <f>SUM(Retail!I:I)</f>
         <v>2012.3240000000001</v>
       </c>
@@ -1895,28 +1915,28 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <f>SUMIF(Business!B:B,B7,Business!D:D) + SUMIF(School!B:B,B7,School!D:D) + SUMIF(Service!B:B,B7,Service!D:D)+SUMIF(Retail!B:B,B7,Retail!D:D) + SUMIF(Tourism!B:B,B7,Tourism!D:D)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="33">
         <f>SUMIF(Business!B:B,B7,Business!I:I) + SUMIF(School!B:B,B7,School!I:I) + SUMIF(Service!B:B,B7,Service!I:I)+SUMIF(Retail!B:B,B7,Retail!I:I) + SUMIF(Tourism!B:B,B7,Tourism!I:I)</f>
         <v>0</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="15">
+        <v>65</v>
+      </c>
+      <c r="G7" s="14">
         <f>SUM(Tourism!D:D)</f>
         <v>3</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="33">
         <f>SUM(Tourism!I:I)</f>
         <v>1775.58</v>
       </c>
@@ -1930,16 +1950,16 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <f>SUMIF(Business!B:B,B8,Business!D:D) + SUMIF(School!B:B,B8,School!D:D) + SUMIF(Service!B:B,B8,Service!D:D)+SUMIF(Retail!B:B,B8,Retail!D:D) + SUMIF(Tourism!B:B,B8,Tourism!D:D)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="33">
         <f>SUMIF(Business!B:B,B8,Business!I:I) + SUMIF(School!B:B,B8,School!I:I) + SUMIF(Service!B:B,B8,Service!I:I)+SUMIF(Retail!B:B,B8,Retail!I:I) + SUMIF(Tourism!B:B,B8,Tourism!I:I)</f>
         <v>0</v>
       </c>
@@ -1947,13 +1967,13 @@
       <c r="F8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>24</v>
-      </c>
-      <c r="H8" s="35">
+        <v>25.5</v>
+      </c>
+      <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>10014.238000000001</v>
+        <v>10724.463</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -1965,23 +1985,23 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <f>SUMIF(Business!B:B,B9,Business!D:D) + SUMIF(School!B:B,B9,School!D:D) + SUMIF(Service!B:B,B9,Service!D:D)+SUMIF(Retail!B:B,B9,Retail!D:D) + SUMIF(Tourism!B:B,B9,Tourism!D:D)</f>
         <v>4</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="33">
         <f>SUMIF(Business!B:B,B9,Business!I:I) + SUMIF(School!B:B,B9,School!I:I) + SUMIF(Service!B:B,B9,Service!I:I)+SUMIF(Retail!B:B,B9,Retail!I:I) + SUMIF(Tourism!B:B,B9,Tourism!I:I)</f>
         <v>1893.9520000000002</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="5"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1992,23 +2012,23 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>24</v>
-      </c>
-      <c r="D10" s="35">
+        <v>25.5</v>
+      </c>
+      <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>10014.238000000001</v>
+        <v>10724.463</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
       <c r="I10" s="5"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -2019,11 +2039,11 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="4"/>
@@ -2035,11 +2055,11 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="4"/>
@@ -2051,15 +2071,15 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="5"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
       <c r="I13" s="5"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -2070,15 +2090,15 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
       <c r="I14" s="5"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2089,15 +2109,15 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -2108,15 +2128,15 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="5"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
       <c r="I16" s="5"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -2127,15 +2147,15 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="5"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2146,15 +2166,15 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="5"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
       <c r="I18" s="5"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -2167,8 +2187,9 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2179,204 +2200,214 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="66" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="67" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="67" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="68" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="58" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="64" style="69" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="66" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="66" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="67" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="57" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64" style="68" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="71" t="s">
+      <c r="F1" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="57" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="59" t="s">
+      <c r="J1" s="56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="73">
+      <c r="D2" s="72">
         <v>5</v>
       </c>
-      <c r="E2" s="62">
+      <c r="E2" s="61">
         <f>IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
         <v>4</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="61">
         <f>IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
         <v>1</v>
       </c>
-      <c r="G2" s="63">
+      <c r="G2" s="62">
         <f>INDEX(CostPerHour,E2)</f>
         <v>355.11</v>
       </c>
-      <c r="H2" s="64">
+      <c r="H2" s="63">
         <f>IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
         <v>1</v>
       </c>
-      <c r="I2" s="63">
+      <c r="I2" s="62">
         <f>D2*G2*H2</f>
         <v>1775.5500000000002</v>
       </c>
-      <c r="J2" s="65" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="62">
+      <c r="J2" s="64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="72">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="61">
         <f>IF(ISERROR(MATCH(C3,SkillList,0)),0,MATCH(C3,SkillList,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="62">
+        <v>1</v>
+      </c>
+      <c r="F3" s="61">
         <f>IF(ISERROR(MATCH(B3,MemberList,0)),0,MATCH(B3,MemberList,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="63">
+        <v>1</v>
+      </c>
+      <c r="G3" s="62">
         <f>INDEX(CostPerHour,E3)</f>
-        <v>946.97</v>
-      </c>
-      <c r="H3" s="64">
+        <v>1183.71</v>
+      </c>
+      <c r="H3" s="63">
         <f>IF(ISERROR(INDEX(Competency,F3,E3)), 0, INDEX(Competency,F3,E3))</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="63">
+        <v>1</v>
+      </c>
+      <c r="I3" s="62">
         <f t="shared" ref="I3:I6" si="0">D3*G3*H3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="65"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="62">
+        <v>591.85500000000002</v>
+      </c>
+      <c r="J3" s="64" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="61">
         <f>IF(ISERROR(MATCH(C4,SkillList,0)),0,MATCH(C4,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F4" s="62">
+      <c r="F4" s="61">
         <f>IF(ISERROR(MATCH(B4,MemberList,0)),0,MATCH(B4,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G4" s="63">
+      <c r="G4" s="62">
         <f>INDEX(CostPerHour,E4)</f>
         <v>946.97</v>
       </c>
-      <c r="H4" s="64">
+      <c r="H4" s="63">
         <f>IF(ISERROR(INDEX(Competency,F4,E4)), 0, INDEX(Competency,F4,E4))</f>
         <v>1</v>
       </c>
-      <c r="I4" s="63">
+      <c r="I4" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J4" s="65"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="62">
+      <c r="J4" s="64"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="61">
         <f>IF(ISERROR(MATCH(C5,SkillList,0)),0,MATCH(C5,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F5" s="62">
+      <c r="F5" s="61">
         <f>IF(ISERROR(MATCH(B5,MemberList,0)),0,MATCH(B5,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="62">
         <f>INDEX(CostPerHour,E5)</f>
         <v>355.11</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="63">
         <f>IF(ISERROR(INDEX(Competency,F5,E5)), 0, INDEX(Competency,F5,E5))</f>
         <v>0</v>
       </c>
-      <c r="I5" s="63">
+      <c r="I5" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="65"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="62">
+      <c r="J5" s="64"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="61">
         <f>IF(ISERROR(MATCH(C6,SkillList,0)),0,MATCH(C6,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F6" s="62">
+      <c r="F6" s="61">
         <f>IF(ISERROR(MATCH(B6,MemberList,0)),0,MATCH(B6,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G6" s="63">
+      <c r="G6" s="62">
         <f>INDEX(CostPerHour,E6)</f>
         <v>355.11</v>
       </c>
-      <c r="H6" s="64">
+      <c r="H6" s="63">
         <f>IF(ISERROR(INDEX(Competency,F6,E6)), 0, INDEX(Competency,F6,E6))</f>
         <v>0</v>
       </c>
-      <c r="I6" s="63">
+      <c r="I6" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="65"/>
+      <c r="J6" s="64"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -2393,210 +2424,210 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="66" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="67" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="67" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="68" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="58" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="64" style="69" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="1" width="10.7109375" style="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="66" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="66" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="67" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="57" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64" style="68" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="55" t="s">
+      <c r="F1" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="57" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="59">
+      <c r="J1" s="56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="58">
         <v>42298</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="61">
+      <c r="D2" s="60">
         <v>2</v>
       </c>
-      <c r="E2" s="62">
+      <c r="E2" s="61">
         <f>IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
         <v>7</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="61">
         <f>IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
         <v>7</v>
       </c>
-      <c r="G2" s="63">
+      <c r="G2" s="62">
         <f>INDEX(CostPerHour,E2)</f>
         <v>591.86</v>
       </c>
-      <c r="H2" s="64">
+      <c r="H2" s="63">
         <f>IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
         <v>0.8</v>
       </c>
-      <c r="I2" s="63">
+      <c r="I2" s="62">
         <f>D2*G2*H2</f>
         <v>946.97600000000011</v>
       </c>
-      <c r="J2" s="65"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="59">
+      <c r="J2" s="64"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="58">
         <v>42299</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="61">
+      <c r="D3" s="60">
         <v>2</v>
       </c>
-      <c r="E3" s="62">
+      <c r="E3" s="61">
         <f>IF(ISERROR(MATCH(C3,SkillList,0)),0,MATCH(C3,SkillList,0))</f>
         <v>7</v>
       </c>
-      <c r="F3" s="62">
+      <c r="F3" s="61">
         <f>IF(ISERROR(MATCH(B3,MemberList,0)),0,MATCH(B3,MemberList,0))</f>
         <v>7</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="62">
         <f>INDEX(CostPerHour,E3)</f>
         <v>591.86</v>
       </c>
-      <c r="H3" s="64">
+      <c r="H3" s="63">
         <f>IF(ISERROR(INDEX(Competency,F3,E3)), 0, INDEX(Competency,F3,E3))</f>
         <v>0.8</v>
       </c>
-      <c r="I3" s="63">
+      <c r="I3" s="62">
         <f t="shared" ref="I3:I6" si="0">D3*G3*H3</f>
         <v>946.97600000000011</v>
       </c>
-      <c r="J3" s="65"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="62">
+      <c r="J3" s="64"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="61">
         <f>IF(ISERROR(MATCH(C4,SkillList,0)),0,MATCH(C4,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F4" s="62">
+      <c r="F4" s="61">
         <f>IF(ISERROR(MATCH(B4,MemberList,0)),0,MATCH(B4,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G4" s="63">
+      <c r="G4" s="62">
         <f>INDEX(CostPerHour,E4)</f>
         <v>946.97</v>
       </c>
-      <c r="H4" s="64">
+      <c r="H4" s="63">
         <f>IF(ISERROR(INDEX(Competency,F4,E4)), 0, INDEX(Competency,F4,E4))</f>
         <v>1</v>
       </c>
-      <c r="I4" s="63">
+      <c r="I4" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J4" s="65"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62">
+      <c r="J4" s="64"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61">
         <f>IF(ISERROR(MATCH(C5,SkillList,0)),0,MATCH(C5,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F5" s="62">
+      <c r="F5" s="61">
         <f>IF(ISERROR(MATCH(B5,MemberList,0)),0,MATCH(B5,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="62">
         <f>INDEX(CostPerHour,E5)</f>
         <v>355.11</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="63">
         <f>IF(ISERROR(INDEX(Competency,F5,E5)), 0, INDEX(Competency,F5,E5))</f>
         <v>0</v>
       </c>
-      <c r="I5" s="63">
+      <c r="I5" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="65"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="62">
+      <c r="J5" s="64"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61">
         <f>IF(ISERROR(MATCH(C6,SkillList,0)),0,MATCH(C6,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F6" s="62">
+      <c r="F6" s="61">
         <f>IF(ISERROR(MATCH(B6,MemberList,0)),0,MATCH(B6,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G6" s="63">
+      <c r="G6" s="62">
         <f>INDEX(CostPerHour,E6)</f>
         <v>355.11</v>
       </c>
-      <c r="H6" s="64">
+      <c r="H6" s="63">
         <f>IF(ISERROR(INDEX(Competency,F6,E6)), 0, INDEX(Competency,F6,E6))</f>
         <v>0</v>
       </c>
-      <c r="I6" s="63">
+      <c r="I6" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="65"/>
+      <c r="J6" s="64"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2612,222 +2643,256 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="66" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="67" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="67" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="68" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="58" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="64" style="69" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="66" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="66" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="67" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="57" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64" style="68" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="55" t="s">
+      <c r="F1" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="57" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="59"/>
-      <c r="B2" s="60" t="s">
+      <c r="J1" s="56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="58"/>
+      <c r="B2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="62">
+      <c r="D2" s="60"/>
+      <c r="E2" s="61">
         <f>IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
         <v>8</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="61">
         <f>IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
         <v>3</v>
       </c>
-      <c r="G2" s="63">
+      <c r="G2" s="62">
         <f>INDEX(CostPerHour,E2)</f>
         <v>236.74</v>
       </c>
-      <c r="H2" s="64">
+      <c r="H2" s="63">
         <f>IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
         <v>0</v>
       </c>
-      <c r="I2" s="63">
+      <c r="I2" s="62">
         <f>D2*G2*H2</f>
         <v>0</v>
       </c>
-      <c r="J2" s="65"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60" t="s">
+      <c r="J2" s="64"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="58"/>
+      <c r="B3" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="62">
+      <c r="D3" s="60"/>
+      <c r="E3" s="61">
         <f>IF(ISERROR(MATCH(C3,SkillList,0)),0,MATCH(C3,SkillList,0))</f>
         <v>8</v>
       </c>
-      <c r="F3" s="62">
+      <c r="F3" s="61">
         <f>IF(ISERROR(MATCH(B3,MemberList,0)),0,MATCH(B3,MemberList,0))</f>
         <v>3</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="62">
         <f>INDEX(CostPerHour,E3)</f>
         <v>236.74</v>
       </c>
-      <c r="H3" s="64">
+      <c r="H3" s="63">
         <f>IF(ISERROR(INDEX(Competency,F3,E3)), 0, INDEX(Competency,F3,E3))</f>
         <v>0</v>
       </c>
-      <c r="I3" s="63">
-        <f t="shared" ref="I3:I6" si="0">D3*G3*H3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="65"/>
-    </row>
-    <row r="4" spans="1:10" ht="30">
-      <c r="A4" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="60" t="s">
+      <c r="I3" s="62">
+        <f t="shared" ref="I3:I8" si="0">D3*G3*H3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="64"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="61">
+      <c r="D4" s="60">
         <v>4</v>
       </c>
-      <c r="E4" s="62">
+      <c r="E4" s="61">
         <f>IF(ISERROR(MATCH(C4,SkillList,0)),0,MATCH(C4,SkillList,0))</f>
         <v>10</v>
       </c>
-      <c r="F4" s="62">
+      <c r="F4" s="61">
         <f>IF(ISERROR(MATCH(B4,MemberList,0)),0,MATCH(B4,MemberList,0))</f>
         <v>1</v>
       </c>
-      <c r="G4" s="63">
+      <c r="G4" s="62">
         <f>INDEX(CostPerHour,E4)</f>
         <v>591.86</v>
       </c>
-      <c r="H4" s="64">
+      <c r="H4" s="63">
         <f>IF(ISERROR(INDEX(Competency,F4,E4)), 0, INDEX(Competency,F4,E4))</f>
         <v>1</v>
       </c>
-      <c r="I4" s="63">
+      <c r="I4" s="62">
         <f t="shared" si="0"/>
         <v>2367.44</v>
       </c>
-      <c r="J4" s="65" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="60" t="s">
+      <c r="J4" s="64" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="61">
+      <c r="D5" s="60">
         <v>4</v>
       </c>
-      <c r="E5" s="62">
+      <c r="E5" s="61">
         <f>IF(ISERROR(MATCH(C5,SkillList,0)),0,MATCH(C5,SkillList,0))</f>
         <v>8</v>
       </c>
-      <c r="F5" s="62">
+      <c r="F5" s="61">
         <f>IF(ISERROR(MATCH(B5,MemberList,0)),0,MATCH(B5,MemberList,0))</f>
         <v>2</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="62">
         <f>INDEX(CostPerHour,E5)</f>
         <v>236.74</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="63">
         <f>IF(ISERROR(INDEX(Competency,F5,E5)), 0, INDEX(Competency,F5,E5))</f>
         <v>0.2</v>
       </c>
-      <c r="I5" s="63">
+      <c r="I5" s="62">
         <f t="shared" si="0"/>
         <v>189.39200000000002</v>
       </c>
-      <c r="J5" s="65" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="62">
+      <c r="J5" s="64" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="60">
+        <v>1</v>
+      </c>
+      <c r="E6" s="61">
         <f>IF(ISERROR(MATCH(C6,SkillList,0)),0,MATCH(C6,SkillList,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="62">
+        <v>8</v>
+      </c>
+      <c r="F6" s="61">
         <f>IF(ISERROR(MATCH(B6,MemberList,0)),0,MATCH(B6,MemberList,0))</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="63">
+        <v>1</v>
+      </c>
+      <c r="G6" s="62">
         <f>INDEX(CostPerHour,E6)</f>
-        <v>355.11</v>
-      </c>
-      <c r="H6" s="64">
+        <v>236.74</v>
+      </c>
+      <c r="H6" s="63">
         <f>IF(ISERROR(INDEX(Competency,F6,E6)), 0, INDEX(Competency,F6,E6))</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="65"/>
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="62">
+        <f t="shared" ref="I6" si="1">D6*G6*H6</f>
+        <v>118.37</v>
+      </c>
+      <c r="J6" s="64" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="58"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="64"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="64"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2843,224 +2908,224 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="66" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="67" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="67" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="68" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="58" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="64" style="69" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="66" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="66" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="67" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="57" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64" style="68" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="55" t="s">
+      <c r="F1" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="57" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="59" t="s">
+      <c r="J1" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="60" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="61">
+      <c r="D2" s="60">
         <v>1</v>
       </c>
-      <c r="E2" s="62">
+      <c r="E2" s="61">
         <f>IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
         <v>7</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="61">
         <f>IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
         <v>2</v>
       </c>
-      <c r="G2" s="63">
+      <c r="G2" s="62">
         <f>INDEX(CostPerHour,E2)</f>
         <v>591.86</v>
       </c>
-      <c r="H2" s="64">
+      <c r="H2" s="63">
         <f>IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
         <v>0.8</v>
       </c>
-      <c r="I2" s="63">
+      <c r="I2" s="62">
         <f>D2*G2*H2</f>
         <v>473.48800000000006</v>
       </c>
-      <c r="J2" s="65" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="60" t="s">
+      <c r="J2" s="64" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="61">
+      <c r="D3" s="60">
         <v>1</v>
       </c>
-      <c r="E3" s="62">
+      <c r="E3" s="61">
         <f>IF(ISERROR(MATCH(C3,SkillList,0)),0,MATCH(C3,SkillList,0))</f>
         <v>7</v>
       </c>
-      <c r="F3" s="62">
+      <c r="F3" s="61">
         <f>IF(ISERROR(MATCH(B3,MemberList,0)),0,MATCH(B3,MemberList,0))</f>
         <v>1</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="62">
         <f>INDEX(CostPerHour,E3)</f>
         <v>591.86</v>
       </c>
-      <c r="H3" s="64">
+      <c r="H3" s="63">
         <f>IF(ISERROR(INDEX(Competency,F3,E3)), 0, INDEX(Competency,F3,E3))</f>
         <v>1</v>
       </c>
-      <c r="I3" s="63">
+      <c r="I3" s="62">
         <f t="shared" ref="I3:I6" si="0">D3*G3*H3</f>
         <v>591.86</v>
       </c>
-      <c r="J3" s="65" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="60" t="s">
+      <c r="J3" s="64" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="61">
+      <c r="D4" s="60">
         <v>2</v>
       </c>
-      <c r="E4" s="62">
+      <c r="E4" s="61">
         <f>IF(ISERROR(MATCH(C4,SkillList,0)),0,MATCH(C4,SkillList,0))</f>
         <v>7</v>
       </c>
-      <c r="F4" s="62">
+      <c r="F4" s="61">
         <f>IF(ISERROR(MATCH(B4,MemberList,0)),0,MATCH(B4,MemberList,0))</f>
         <v>2</v>
       </c>
-      <c r="G4" s="63">
+      <c r="G4" s="62">
         <f>INDEX(CostPerHour,E4)</f>
         <v>591.86</v>
       </c>
-      <c r="H4" s="64">
+      <c r="H4" s="63">
         <f>IF(ISERROR(INDEX(Competency,F4,E4)), 0, INDEX(Competency,F4,E4))</f>
         <v>0.8</v>
       </c>
-      <c r="I4" s="63">
+      <c r="I4" s="62">
         <f t="shared" si="0"/>
         <v>946.97600000000011</v>
       </c>
-      <c r="J4" s="65" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62">
+      <c r="J4" s="64" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61">
         <f>IF(ISERROR(MATCH(C5,SkillList,0)),0,MATCH(C5,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F5" s="62">
+      <c r="F5" s="61">
         <f>IF(ISERROR(MATCH(B5,MemberList,0)),0,MATCH(B5,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="62">
         <f>INDEX(CostPerHour,E5)</f>
         <v>355.11</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="63">
         <f>IF(ISERROR(INDEX(Competency,F5,E5)), 0, INDEX(Competency,F5,E5))</f>
         <v>0</v>
       </c>
-      <c r="I5" s="63">
+      <c r="I5" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="65"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="62">
+      <c r="J5" s="64"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61">
         <f>IF(ISERROR(MATCH(C6,SkillList,0)),0,MATCH(C6,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F6" s="62">
+      <c r="F6" s="61">
         <f>IF(ISERROR(MATCH(B6,MemberList,0)),0,MATCH(B6,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G6" s="63">
+      <c r="G6" s="62">
         <f>INDEX(CostPerHour,E6)</f>
         <v>355.11</v>
       </c>
-      <c r="H6" s="64">
+      <c r="H6" s="63">
         <f>IF(ISERROR(INDEX(Competency,F6,E6)), 0, INDEX(Competency,F6,E6))</f>
         <v>0</v>
       </c>
-      <c r="I6" s="63">
+      <c r="I6" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="65"/>
+      <c r="J6" s="64"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -3076,204 +3141,204 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="66" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="67" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="67" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="68" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="58" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="64" style="69" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="66" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="66" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="67" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="57" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64" style="68" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="55" t="s">
+      <c r="F1" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="57" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="60" t="s">
+      <c r="J1" s="56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="61">
+      <c r="D2" s="60">
         <v>3</v>
       </c>
-      <c r="E2" s="62">
+      <c r="E2" s="61">
         <f>IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
         <v>7</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="61">
         <f>IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
         <v>1</v>
       </c>
-      <c r="G2" s="63">
+      <c r="G2" s="62">
         <f>INDEX(CostPerHour,E2)</f>
         <v>591.86</v>
       </c>
-      <c r="H2" s="64">
+      <c r="H2" s="63">
         <f>IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
         <v>1</v>
       </c>
-      <c r="I2" s="63">
+      <c r="I2" s="62">
         <f>D2*G2*H2</f>
         <v>1775.58</v>
       </c>
-      <c r="J2" s="65" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="62">
+      <c r="J2" s="64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="58"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="61">
         <f>IF(ISERROR(MATCH(C3,SkillList,0)),0,MATCH(C3,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F3" s="62">
+      <c r="F3" s="61">
         <f>IF(ISERROR(MATCH(B3,MemberList,0)),0,MATCH(B3,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="62">
         <f>INDEX(CostPerHour,E3)</f>
         <v>946.97</v>
       </c>
-      <c r="H3" s="64">
+      <c r="H3" s="63">
         <f>IF(ISERROR(INDEX(Competency,F3,E3)), 0, INDEX(Competency,F3,E3))</f>
         <v>0</v>
       </c>
-      <c r="I3" s="63">
+      <c r="I3" s="62">
         <f t="shared" ref="I3:I6" si="0">D3*G3*H3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="65"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="62">
+      <c r="J3" s="64"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="61">
         <f>IF(ISERROR(MATCH(C4,SkillList,0)),0,MATCH(C4,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F4" s="62">
+      <c r="F4" s="61">
         <f>IF(ISERROR(MATCH(B4,MemberList,0)),0,MATCH(B4,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G4" s="63">
+      <c r="G4" s="62">
         <f>INDEX(CostPerHour,E4)</f>
         <v>946.97</v>
       </c>
-      <c r="H4" s="64">
+      <c r="H4" s="63">
         <f>IF(ISERROR(INDEX(Competency,F4,E4)), 0, INDEX(Competency,F4,E4))</f>
         <v>1</v>
       </c>
-      <c r="I4" s="63">
+      <c r="I4" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J4" s="65"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62">
+      <c r="J4" s="64"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61">
         <f>IF(ISERROR(MATCH(C5,SkillList,0)),0,MATCH(C5,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F5" s="62">
+      <c r="F5" s="61">
         <f>IF(ISERROR(MATCH(B5,MemberList,0)),0,MATCH(B5,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="62">
         <f>INDEX(CostPerHour,E5)</f>
         <v>355.11</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="63">
         <f>IF(ISERROR(INDEX(Competency,F5,E5)), 0, INDEX(Competency,F5,E5))</f>
         <v>0</v>
       </c>
-      <c r="I5" s="63">
+      <c r="I5" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="65"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="62">
+      <c r="J5" s="64"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61">
         <f>IF(ISERROR(MATCH(C6,SkillList,0)),0,MATCH(C6,SkillList,0))</f>
         <v>0</v>
       </c>
-      <c r="F6" s="62">
+      <c r="F6" s="61">
         <f>IF(ISERROR(MATCH(B6,MemberList,0)),0,MATCH(B6,MemberList,0))</f>
         <v>0</v>
       </c>
-      <c r="G6" s="63">
+      <c r="G6" s="62">
         <f>INDEX(CostPerHour,E6)</f>
         <v>355.11</v>
       </c>
-      <c r="H6" s="64">
+      <c r="H6" s="63">
         <f>IF(ISERROR(INDEX(Competency,F6,E6)), 0, INDEX(Competency,F6,E6))</f>
         <v>0</v>
       </c>
-      <c r="I6" s="63">
+      <c r="I6" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="65"/>
+      <c r="J6" s="64"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -3289,14 +3354,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -3309,683 +3374,683 @@
     <col min="30" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="92" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="89" t="s">
+    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="91" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="91"/>
+      <c r="C1" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="90"/>
-      <c r="U1" s="90"/>
-      <c r="V1" s="90"/>
-      <c r="W1" s="90"/>
-      <c r="X1" s="90"/>
-      <c r="Y1" s="90"/>
-      <c r="Z1" s="90"/>
-      <c r="AA1" s="90"/>
-      <c r="AB1" s="90"/>
-      <c r="AC1" s="90"/>
-      <c r="AD1" s="90"/>
-      <c r="AE1" s="90"/>
-      <c r="AF1" s="90"/>
-      <c r="AG1" s="90"/>
-      <c r="AH1" s="90"/>
-      <c r="AI1" s="91"/>
-    </row>
-    <row r="2" spans="1:35" s="27" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="93"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="94" t="s">
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+      <c r="X1" s="89"/>
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="89"/>
+      <c r="AA1" s="89"/>
+      <c r="AB1" s="89"/>
+      <c r="AC1" s="89"/>
+      <c r="AD1" s="89"/>
+      <c r="AE1" s="89"/>
+      <c r="AF1" s="89"/>
+      <c r="AG1" s="89"/>
+      <c r="AH1" s="89"/>
+      <c r="AI1" s="90"/>
+    </row>
+    <row r="2" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="94" t="s">
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="95" t="s">
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="95"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="95"/>
-      <c r="V2" s="95"/>
-      <c r="W2" s="95"/>
-      <c r="X2" s="95"/>
-      <c r="Y2" s="95"/>
-      <c r="Z2" s="95"/>
-      <c r="AA2" s="96"/>
-      <c r="AB2" s="97" t="s">
+      <c r="S2" s="94"/>
+      <c r="T2" s="94"/>
+      <c r="U2" s="94"/>
+      <c r="V2" s="94"/>
+      <c r="W2" s="94"/>
+      <c r="X2" s="94"/>
+      <c r="Y2" s="94"/>
+      <c r="Z2" s="94"/>
+      <c r="AA2" s="95"/>
+      <c r="AB2" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="98"/>
-      <c r="AD2" s="98"/>
-      <c r="AE2" s="99"/>
-      <c r="AF2" s="86" t="s">
+      <c r="AC2" s="97"/>
+      <c r="AD2" s="97"/>
+      <c r="AE2" s="98"/>
+      <c r="AF2" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="AG2" s="87"/>
-      <c r="AH2" s="87"/>
-      <c r="AI2" s="88"/>
-    </row>
-    <row r="3" spans="1:35" ht="180">
+      <c r="AG2" s="86"/>
+      <c r="AH2" s="86"/>
+      <c r="AI2" s="87"/>
+    </row>
+    <row r="3" spans="1:35" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="51" t="s">
+      <c r="O3" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="51" t="s">
+      <c r="P3" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="R3" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="U3" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="V3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="W3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z3" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB3" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC3" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="Q3" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="R3" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="U3" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="V3" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="W3" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y3" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z3" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA3" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB3" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC3" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD3" s="25" t="s">
+      <c r="AD3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="AE3" s="43" t="s">
+      <c r="AE3" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="AF3" s="42" t="s">
+      <c r="AF3" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="AG3" s="25" t="s">
+      <c r="AG3" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AH3" s="25" t="s">
+      <c r="AH3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="AI3" s="43" t="s">
+      <c r="AI3" s="42" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
-      <c r="A4" s="24">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
         <v>1</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="43">
         <v>1</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="35">
         <v>1</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="35">
         <v>1</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="35">
         <v>1</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>1</v>
       </c>
-      <c r="H4" s="45">
+      <c r="H4" s="44">
         <v>1</v>
       </c>
-      <c r="I4" s="44">
+      <c r="I4" s="43">
         <v>1</v>
       </c>
-      <c r="J4" s="36">
+      <c r="J4" s="35">
         <v>0.5</v>
       </c>
-      <c r="K4" s="36">
+      <c r="K4" s="35">
         <v>1</v>
       </c>
-      <c r="L4" s="36">
+      <c r="L4" s="35">
         <v>1</v>
       </c>
-      <c r="M4" s="36">
+      <c r="M4" s="35">
         <v>1</v>
       </c>
-      <c r="N4" s="36">
+      <c r="N4" s="35">
         <v>1</v>
       </c>
-      <c r="O4" s="52">
+      <c r="O4" s="51">
         <v>0.8</v>
       </c>
-      <c r="P4" s="45">
+      <c r="P4" s="44">
         <v>1</v>
       </c>
-      <c r="Q4" s="45">
+      <c r="Q4" s="44">
         <v>0.8</v>
       </c>
-      <c r="R4" s="40">
-        <v>0</v>
-      </c>
-      <c r="S4" s="36">
-        <v>0</v>
-      </c>
-      <c r="T4" s="36">
+      <c r="R4" s="39">
+        <v>0</v>
+      </c>
+      <c r="S4" s="35">
+        <v>0</v>
+      </c>
+      <c r="T4" s="35">
         <v>1</v>
       </c>
-      <c r="U4" s="36">
+      <c r="U4" s="35">
         <v>1</v>
       </c>
-      <c r="V4" s="36">
-        <v>0</v>
-      </c>
-      <c r="W4" s="36">
-        <v>0</v>
-      </c>
-      <c r="X4" s="36">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="36">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="45">
+      <c r="V4" s="35">
+        <v>0</v>
+      </c>
+      <c r="W4" s="35">
+        <v>0</v>
+      </c>
+      <c r="X4" s="35">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="35">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="44">
         <v>1</v>
       </c>
-      <c r="AB4" s="44">
+      <c r="AB4" s="43">
         <v>1</v>
       </c>
-      <c r="AC4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="36">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="45">
+      <c r="AC4" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="35">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="44">
         <v>1</v>
       </c>
-      <c r="AF4" s="44">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="36">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="36">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35">
-      <c r="A5" s="24">
+      <c r="AF4" s="43">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="35">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
         <v>2</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>0.5</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="36">
         <v>0.2</v>
       </c>
-      <c r="E5" s="37">
-        <v>0</v>
-      </c>
-      <c r="F5" s="37">
-        <v>0</v>
-      </c>
-      <c r="G5" s="37">
-        <v>0</v>
-      </c>
-      <c r="H5" s="47">
-        <v>0</v>
-      </c>
-      <c r="I5" s="46">
+      <c r="E5" s="36">
+        <v>0</v>
+      </c>
+      <c r="F5" s="36">
+        <v>0</v>
+      </c>
+      <c r="G5" s="36">
+        <v>0</v>
+      </c>
+      <c r="H5" s="46">
+        <v>0</v>
+      </c>
+      <c r="I5" s="45">
         <v>0.8</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="36">
         <v>0.2</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="36">
         <v>0.5</v>
       </c>
-      <c r="L5" s="37">
+      <c r="L5" s="36">
         <v>0.3</v>
       </c>
-      <c r="M5" s="37">
+      <c r="M5" s="36">
         <v>1</v>
       </c>
-      <c r="N5" s="37">
+      <c r="N5" s="36">
         <v>1</v>
       </c>
-      <c r="O5" s="53">
+      <c r="O5" s="52">
         <v>0.5</v>
       </c>
-      <c r="P5" s="53">
+      <c r="P5" s="52">
         <v>0.8</v>
       </c>
-      <c r="Q5" s="47">
+      <c r="Q5" s="46">
         <v>0.5</v>
       </c>
-      <c r="R5" s="41">
-        <v>0</v>
-      </c>
-      <c r="S5" s="37">
-        <v>0</v>
-      </c>
-      <c r="T5" s="36">
-        <v>0</v>
-      </c>
-      <c r="U5" s="36">
-        <v>0</v>
-      </c>
-      <c r="V5" s="36">
-        <v>0</v>
-      </c>
-      <c r="W5" s="36">
-        <v>0</v>
-      </c>
-      <c r="X5" s="36">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="36">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="44">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="36">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="44">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="36">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="36">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35">
-      <c r="A6" s="24">
+      <c r="R5" s="40">
+        <v>0</v>
+      </c>
+      <c r="S5" s="36">
+        <v>0</v>
+      </c>
+      <c r="T5" s="35">
+        <v>0</v>
+      </c>
+      <c r="U5" s="35">
+        <v>0</v>
+      </c>
+      <c r="V5" s="35">
+        <v>0</v>
+      </c>
+      <c r="W5" s="35">
+        <v>0</v>
+      </c>
+      <c r="X5" s="35">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="35">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="43">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="35">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="43">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="35">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
         <v>3</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="36"/>
-      <c r="U6" s="36"/>
-      <c r="V6" s="36"/>
-      <c r="W6" s="36"/>
-      <c r="X6" s="36"/>
-      <c r="Y6" s="36"/>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="45"/>
-      <c r="AB6" s="44"/>
-      <c r="AC6" s="40"/>
-      <c r="AD6" s="36"/>
-      <c r="AE6" s="45"/>
-      <c r="AF6" s="44"/>
-      <c r="AG6" s="36"/>
-      <c r="AH6" s="36"/>
-      <c r="AI6" s="45"/>
-    </row>
-    <row r="7" spans="1:35">
-      <c r="A7" s="24">
+      <c r="C6" s="45"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="44"/>
+      <c r="AB6" s="43"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="35"/>
+      <c r="AE6" s="44"/>
+      <c r="AF6" s="43"/>
+      <c r="AG6" s="35"/>
+      <c r="AH6" s="35"/>
+      <c r="AI6" s="44"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="23">
         <v>4</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="36"/>
-      <c r="V7" s="36"/>
-      <c r="W7" s="36"/>
-      <c r="X7" s="36"/>
-      <c r="Y7" s="36"/>
-      <c r="Z7" s="36"/>
-      <c r="AA7" s="45"/>
-      <c r="AB7" s="44"/>
-      <c r="AC7" s="40"/>
-      <c r="AD7" s="36"/>
-      <c r="AE7" s="45"/>
-      <c r="AF7" s="44"/>
-      <c r="AG7" s="36"/>
-      <c r="AH7" s="36"/>
-      <c r="AI7" s="45"/>
-    </row>
-    <row r="8" spans="1:35">
-      <c r="A8" s="24">
+      <c r="C7" s="45"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
+      <c r="X7" s="35"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="44"/>
+      <c r="AB7" s="43"/>
+      <c r="AC7" s="39"/>
+      <c r="AD7" s="35"/>
+      <c r="AE7" s="44"/>
+      <c r="AF7" s="43"/>
+      <c r="AG7" s="35"/>
+      <c r="AH7" s="35"/>
+      <c r="AI7" s="44"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
         <v>5</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="36"/>
-      <c r="U8" s="36"/>
-      <c r="V8" s="36"/>
-      <c r="W8" s="36"/>
-      <c r="X8" s="36"/>
-      <c r="Y8" s="36"/>
-      <c r="Z8" s="36"/>
-      <c r="AA8" s="45"/>
-      <c r="AB8" s="44"/>
-      <c r="AC8" s="40"/>
-      <c r="AD8" s="36"/>
-      <c r="AE8" s="45"/>
-      <c r="AF8" s="44"/>
-      <c r="AG8" s="36"/>
-      <c r="AH8" s="36"/>
-      <c r="AI8" s="45"/>
-    </row>
-    <row r="9" spans="1:35">
-      <c r="A9" s="24">
+      <c r="C8" s="45"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="35"/>
+      <c r="AA8" s="44"/>
+      <c r="AB8" s="43"/>
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="35"/>
+      <c r="AE8" s="44"/>
+      <c r="AF8" s="43"/>
+      <c r="AG8" s="35"/>
+      <c r="AH8" s="35"/>
+      <c r="AI8" s="44"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" s="23">
         <v>6</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="36"/>
-      <c r="U9" s="36"/>
-      <c r="V9" s="36"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="36"/>
-      <c r="Y9" s="36"/>
-      <c r="Z9" s="36"/>
-      <c r="AA9" s="45"/>
-      <c r="AB9" s="44"/>
-      <c r="AC9" s="40"/>
-      <c r="AD9" s="36"/>
-      <c r="AE9" s="45"/>
-      <c r="AF9" s="44"/>
-      <c r="AG9" s="36"/>
-      <c r="AH9" s="36"/>
-      <c r="AI9" s="45"/>
-    </row>
-    <row r="10" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A10" s="24">
+      <c r="C9" s="45"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35"/>
+      <c r="AA9" s="44"/>
+      <c r="AB9" s="43"/>
+      <c r="AC9" s="39"/>
+      <c r="AD9" s="35"/>
+      <c r="AE9" s="44"/>
+      <c r="AF9" s="43"/>
+      <c r="AG9" s="35"/>
+      <c r="AH9" s="35"/>
+      <c r="AI9" s="44"/>
+    </row>
+    <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="23">
         <v>7</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="48">
+      <c r="C10" s="47">
         <v>0.25</v>
       </c>
-      <c r="D10" s="49">
+      <c r="D10" s="48">
         <v>0.25</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="48">
         <v>0.25</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="48">
         <v>0.25</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G10" s="48">
         <v>0.25</v>
       </c>
-      <c r="H10" s="50">
+      <c r="H10" s="49">
         <v>0.25</v>
       </c>
-      <c r="I10" s="48">
+      <c r="I10" s="47">
         <v>0.8</v>
       </c>
-      <c r="J10" s="48">
+      <c r="J10" s="47">
         <v>0.5</v>
       </c>
-      <c r="K10" s="48">
+      <c r="K10" s="47">
         <v>0.5</v>
       </c>
-      <c r="L10" s="48">
-        <v>0</v>
-      </c>
-      <c r="M10" s="48">
+      <c r="L10" s="47">
+        <v>0</v>
+      </c>
+      <c r="M10" s="47">
         <v>0.25</v>
       </c>
-      <c r="N10" s="48">
-        <v>0</v>
-      </c>
-      <c r="O10" s="48">
+      <c r="N10" s="47">
+        <v>0</v>
+      </c>
+      <c r="O10" s="47">
         <v>0.5</v>
       </c>
-      <c r="P10" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="48">
-        <v>0</v>
-      </c>
-      <c r="R10" s="48">
+      <c r="P10" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="47">
+        <v>0</v>
+      </c>
+      <c r="R10" s="47">
         <v>0.25</v>
       </c>
-      <c r="S10" s="49">
+      <c r="S10" s="48">
         <v>0.25</v>
       </c>
-      <c r="T10" s="49">
+      <c r="T10" s="48">
         <v>0.5</v>
       </c>
-      <c r="U10" s="48">
-        <v>0</v>
-      </c>
-      <c r="V10" s="48">
+      <c r="U10" s="47">
+        <v>0</v>
+      </c>
+      <c r="V10" s="47">
         <v>0.5</v>
       </c>
-      <c r="W10" s="48">
+      <c r="W10" s="47">
         <v>0.5</v>
       </c>
-      <c r="X10" s="48">
+      <c r="X10" s="47">
         <v>0.25</v>
       </c>
-      <c r="Y10" s="48">
+      <c r="Y10" s="47">
         <v>0.25</v>
       </c>
-      <c r="Z10" s="48">
+      <c r="Z10" s="47">
         <v>0.25</v>
       </c>
-      <c r="AA10" s="48">
+      <c r="AA10" s="47">
         <v>1</v>
       </c>
-      <c r="AB10" s="48">
+      <c r="AB10" s="47">
         <v>0.25</v>
       </c>
-      <c r="AC10" s="48">
+      <c r="AC10" s="47">
         <v>0.25</v>
       </c>
-      <c r="AD10" s="48">
+      <c r="AD10" s="47">
         <v>0.25</v>
       </c>
-      <c r="AE10" s="48">
+      <c r="AE10" s="47">
         <v>0.5</v>
       </c>
-      <c r="AF10" s="48">
+      <c r="AF10" s="47">
         <v>0.25</v>
       </c>
-      <c r="AG10" s="48">
+      <c r="AG10" s="47">
         <v>1</v>
       </c>
-      <c r="AH10" s="48">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="48">
+      <c r="AH10" s="47">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="47">
         <v>0</v>
       </c>
     </row>
@@ -4005,26 +4070,24 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15" style="33" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15" style="32" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>5</v>
@@ -4032,21 +4095,21 @@
       <c r="C1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>53</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="100" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="99" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="9">
@@ -4055,150 +4118,150 @@
       <c r="C2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="33">
         <v>10000000</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="33">
         <f>D2/4</f>
         <v>2500000</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <f>E2/12</f>
         <v>208333.33333333334</v>
       </c>
-      <c r="G2" s="34">
+      <c r="G2" s="33">
         <f>ROUND(F2/22/8,2)</f>
         <v>1183.71</v>
       </c>
-      <c r="H2" s="74"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="101"/>
+      <c r="H2" s="73"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="100"/>
       <c r="B3" s="9">
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D3" s="33">
         <v>8000000</v>
       </c>
-      <c r="E3" s="34">
+      <c r="E3" s="33">
         <f t="shared" ref="E3:E34" si="0">D3/4</f>
         <v>2000000</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <f t="shared" ref="F3:F34" si="1">E3/12</f>
         <v>166666.66666666666</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G3" s="33">
         <f t="shared" ref="G3:G34" si="2">ROUND(F3/22/8,2)</f>
         <v>946.97</v>
       </c>
-      <c r="H3" s="74"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="101"/>
+      <c r="H3" s="73"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="100"/>
       <c r="B4" s="9">
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="33">
         <v>8000000</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="33">
         <f t="shared" si="0"/>
         <v>2000000</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <f t="shared" si="1"/>
         <v>166666.66666666666</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="33">
         <f t="shared" si="2"/>
         <v>946.97</v>
       </c>
-      <c r="H4" s="74"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="101"/>
+      <c r="H4" s="73"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="100"/>
       <c r="B5" s="9">
         <v>4</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="33">
         <v>3000000</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="33">
         <f t="shared" si="0"/>
         <v>750000</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <f t="shared" si="1"/>
         <v>62500</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="33">
         <f t="shared" si="2"/>
         <v>355.11</v>
       </c>
-      <c r="H5" s="74"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="101"/>
+      <c r="H5" s="73"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="100"/>
       <c r="B6" s="9">
         <v>5</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="33">
         <v>3000000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="33">
         <f t="shared" si="0"/>
         <v>750000</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <f t="shared" si="1"/>
         <v>62500</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="33">
         <f t="shared" si="2"/>
         <v>355.11</v>
       </c>
-      <c r="H6" s="74"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="102"/>
+      <c r="H6" s="73"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="101"/>
       <c r="B7" s="9">
         <v>6</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="33">
         <v>8000000</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="33">
         <f t="shared" si="0"/>
         <v>2000000</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <f t="shared" si="1"/>
         <v>166666.66666666666</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="33">
         <f t="shared" si="2"/>
         <v>946.97</v>
       </c>
-      <c r="H7" s="74"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="100" t="s">
+      <c r="H7" s="73"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="99" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="9">
@@ -4207,217 +4270,217 @@
       <c r="C8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="33">
         <v>5000000</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="33">
         <f t="shared" si="0"/>
         <v>1250000</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <f t="shared" si="1"/>
         <v>104166.66666666667</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="33">
         <f t="shared" si="2"/>
         <v>591.86</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="101"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="100"/>
       <c r="B9" s="9">
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="33">
         <v>2000000</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="33">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <f t="shared" si="1"/>
         <v>41666.666666666664</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="33">
         <f t="shared" si="2"/>
         <v>236.74</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="101"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="100"/>
       <c r="B10" s="9">
         <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="33">
         <v>1500000</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="33">
         <f t="shared" si="0"/>
         <v>375000</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <f t="shared" si="1"/>
         <v>31250</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="33">
         <f t="shared" si="2"/>
         <v>177.56</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="101"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="100"/>
       <c r="B11" s="9">
         <v>10</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="33">
         <v>5000000</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="33">
         <f t="shared" si="0"/>
         <v>1250000</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <f t="shared" si="1"/>
         <v>104166.66666666667</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="33">
         <f t="shared" si="2"/>
         <v>591.86</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="101"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="100"/>
       <c r="B12" s="9">
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="33">
         <v>1500000</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="33">
         <f t="shared" si="0"/>
         <v>375000</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <f t="shared" si="1"/>
         <v>31250</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="33">
         <f t="shared" si="2"/>
         <v>177.56</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="101"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="100"/>
       <c r="B13" s="9">
         <v>12</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="33">
         <v>1000000</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="33">
         <f t="shared" si="0"/>
         <v>250000</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <f t="shared" si="1"/>
         <v>20833.333333333332</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="33">
         <f t="shared" si="2"/>
         <v>118.37</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="101"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="100"/>
       <c r="B14" s="9">
         <v>13</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="33">
         <v>1000000</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="33">
         <f t="shared" si="0"/>
         <v>250000</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <f t="shared" si="1"/>
         <v>20833.333333333332</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="33">
         <f t="shared" si="2"/>
         <v>118.37</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="101"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="100"/>
       <c r="B15" s="9">
         <v>14</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="34">
+        <v>71</v>
+      </c>
+      <c r="D15" s="33">
         <v>2500000</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="33">
         <f t="shared" si="0"/>
         <v>625000</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <f t="shared" si="1"/>
         <v>52083.333333333336</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="33">
         <f t="shared" si="2"/>
         <v>295.93</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="101"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="100"/>
       <c r="B16" s="9">
         <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="34">
+        <v>70</v>
+      </c>
+      <c r="D16" s="33">
         <v>1000000</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="33">
         <f t="shared" si="0"/>
         <v>250000</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <f t="shared" si="1"/>
         <v>20833.333333333332</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="33">
         <f t="shared" si="2"/>
         <v>118.37</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="100" t="s">
-        <v>69</v>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="99" t="s">
+        <v>67</v>
       </c>
       <c r="B17" s="9">
         <v>16</v>
@@ -4425,241 +4488,241 @@
       <c r="C17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="33">
         <v>1500000</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="33">
         <f t="shared" si="0"/>
         <v>375000</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="14">
         <f t="shared" si="1"/>
         <v>31250</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="33">
         <f t="shared" si="2"/>
         <v>177.56</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="101"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="100"/>
       <c r="B18" s="9">
         <v>17</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="33">
         <v>600000</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="33">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <f t="shared" si="1"/>
         <v>12500</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="33">
         <f t="shared" si="2"/>
         <v>71.02</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="101"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="100"/>
       <c r="B19" s="9">
         <v>18</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="33">
         <v>300000</v>
       </c>
-      <c r="E19" s="34">
+      <c r="E19" s="33">
         <f t="shared" si="0"/>
         <v>75000</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="14">
         <f t="shared" si="1"/>
         <v>6250</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="33">
         <f t="shared" si="2"/>
         <v>35.51</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="101"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="100"/>
       <c r="B20" s="9">
         <v>19</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="34">
+        <v>74</v>
+      </c>
+      <c r="D20" s="33">
         <v>2000000</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="33">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="14">
         <f t="shared" si="1"/>
         <v>41666.666666666664</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="33">
         <f t="shared" si="2"/>
         <v>236.74</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="101"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="100"/>
       <c r="B21" s="9">
         <v>20</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="33">
         <v>600000</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="33">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="14">
         <f t="shared" si="1"/>
         <v>12500</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="33">
         <f t="shared" si="2"/>
         <v>71.02</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="101"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="100"/>
       <c r="B22" s="9">
         <v>21</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D22" s="33">
         <v>300000</v>
       </c>
-      <c r="E22" s="34">
+      <c r="E22" s="33">
         <f t="shared" si="0"/>
         <v>75000</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="14">
         <f t="shared" si="1"/>
         <v>6250</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="33">
         <f t="shared" si="2"/>
         <v>35.51</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="101"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="100"/>
       <c r="B23" s="9">
         <v>22</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="33">
         <v>600000</v>
       </c>
-      <c r="E23" s="34">
+      <c r="E23" s="33">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="14">
         <f t="shared" si="1"/>
         <v>12500</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="33">
         <f t="shared" si="2"/>
         <v>71.02</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="101"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="100"/>
       <c r="B24" s="9">
         <v>23</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24" s="33">
         <v>300000</v>
       </c>
-      <c r="E24" s="34">
+      <c r="E24" s="33">
         <f t="shared" si="0"/>
         <v>75000</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="14">
         <f t="shared" si="1"/>
         <v>6250</v>
       </c>
-      <c r="G24" s="34">
+      <c r="G24" s="33">
         <f t="shared" si="2"/>
         <v>35.51</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="101"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="100"/>
       <c r="B25" s="9">
         <v>24</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="33">
         <v>300000</v>
       </c>
-      <c r="E25" s="34">
+      <c r="E25" s="33">
         <f t="shared" si="0"/>
         <v>75000</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="14">
         <f t="shared" si="1"/>
         <v>6250</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="33">
         <f t="shared" si="2"/>
         <v>35.51</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="102"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="101"/>
       <c r="B26" s="9">
         <v>25</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="33">
         <v>600000</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="33">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="14">
         <f t="shared" si="1"/>
         <v>12500</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="33">
         <f t="shared" si="2"/>
         <v>71.02</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="100" t="s">
-        <v>70</v>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="99" t="s">
+        <v>68</v>
       </c>
       <c r="B27" s="9">
         <v>26</v>
@@ -4667,96 +4730,96 @@
       <c r="C27" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="33">
         <v>2500000</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="33">
         <f t="shared" si="0"/>
         <v>625000</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="14">
         <f t="shared" si="1"/>
         <v>52083.333333333336</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="33">
         <f t="shared" si="2"/>
         <v>295.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="101"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="100"/>
       <c r="B28" s="9">
         <v>27</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="34">
+        <v>73</v>
+      </c>
+      <c r="D28" s="33">
         <v>600000</v>
       </c>
-      <c r="E28" s="34">
+      <c r="E28" s="33">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="14">
         <f t="shared" si="1"/>
         <v>12500</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G28" s="33">
         <f t="shared" si="2"/>
         <v>71.02</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="101"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="100"/>
       <c r="B29" s="9">
         <v>28</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="33">
         <v>1500000</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="33">
         <f t="shared" si="0"/>
         <v>375000</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="14">
         <f t="shared" si="1"/>
         <v>31250</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="33">
         <f t="shared" si="2"/>
         <v>177.56</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="102"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="101"/>
       <c r="B30" s="9">
         <v>29</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="34">
+      <c r="D30" s="33">
         <v>600000</v>
       </c>
-      <c r="E30" s="34">
+      <c r="E30" s="33">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="14">
         <f t="shared" si="1"/>
         <v>12500</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="33">
         <f t="shared" si="2"/>
         <v>71.02</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="100" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="99" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="9">
@@ -4765,95 +4828,96 @@
       <c r="C31" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D31" s="33">
         <v>300000</v>
       </c>
-      <c r="E31" s="34">
+      <c r="E31" s="33">
         <f t="shared" si="0"/>
         <v>75000</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="14">
         <f t="shared" si="1"/>
         <v>6250</v>
       </c>
-      <c r="G31" s="34">
+      <c r="G31" s="33">
         <f t="shared" si="2"/>
         <v>35.51</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="101"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="100"/>
       <c r="B32" s="9">
         <v>31</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="33">
         <v>300000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="33">
         <f t="shared" si="0"/>
         <v>75000</v>
       </c>
-      <c r="F32" s="15">
+      <c r="F32" s="14">
         <f t="shared" si="1"/>
         <v>6250</v>
       </c>
-      <c r="G32" s="34">
+      <c r="G32" s="33">
         <f t="shared" si="2"/>
         <v>35.51</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="101"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="100"/>
       <c r="B33" s="9">
         <v>32</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="34">
+      <c r="D33" s="33">
         <v>600000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="33">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="F33" s="15">
+      <c r="F33" s="14">
         <f t="shared" si="1"/>
         <v>12500</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G33" s="33">
         <f t="shared" si="2"/>
         <v>71.02</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="101"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="100"/>
       <c r="B34" s="9">
         <v>33</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="34">
+      <c r="D34" s="33">
         <v>1000000</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="33">
         <f t="shared" si="0"/>
         <v>250000</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="14">
         <f t="shared" si="1"/>
         <v>20833.333333333332</v>
       </c>
-      <c r="G34" s="34">
+      <c r="G34" s="33">
         <f t="shared" si="2"/>
         <v>118.37</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="5">
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A2:A7"/>

</xml_diff>

<commit_message>
Adding effort on Business analysis for school project
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="8" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="93">
   <si>
     <t>Total</t>
   </si>
@@ -1511,7 +1511,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>10014.231</v>
+        <v>10191.791000000001</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1532,7 +1532,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1553,7 +1553,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>3.1875</v>
+        <v>3.4375</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1827,11 +1827,11 @@
       </c>
       <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
-        <v>1183.72</v>
+        <v>1361.28</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -1967,11 +1967,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>10014.231</v>
+        <v>10191.791000000001</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -1990,11 +1990,11 @@
       </c>
       <c r="C9" s="14">
         <f>SUMIF(Business!B:B,B9,Business!D:D) + SUMIF(School!B:B,B9,School!D:D) + SUMIF(Service!B:B,B9,Service!D:D)+SUMIF(Retail!B:B,B9,Retail!D:D) + SUMIF(Tourism!B:B,B9,Tourism!D:D)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9" s="33">
         <f>SUMIF(Business!B:B,B9,Business!I:I) + SUMIF(School!B:B,B9,School!I:I) + SUMIF(Service!B:B,B9,Service!I:I)+SUMIF(Retail!B:B,B9,Retail!I:I) + SUMIF(Tourism!B:B,B9,Tourism!I:I)</f>
-        <v>1183.72</v>
+        <v>1361.28</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
@@ -2017,11 +2017,11 @@
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>10014.231</v>
+        <v>10191.791000000001</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2425,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2547,29 +2547,37 @@
       <c r="J3" s="64"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
+      <c r="A4" s="58">
+        <v>42301</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="60">
+        <v>2</v>
+      </c>
       <c r="E4" s="61">
         <f>IF(ISERROR(MATCH(C4,SkillList,0)),0,MATCH(C4,SkillList,0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F4" s="61">
         <f>IF(ISERROR(MATCH(B4,MemberList,0)),0,MATCH(B4,MemberList,0))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G4" s="62">
         <f>INDEX(CostPerHour,E4)</f>
-        <v>946.97</v>
+        <v>177.56</v>
       </c>
       <c r="H4" s="63">
         <f>IF(ISERROR(INDEX(Competency,F4,E4)), 0, INDEX(Competency,F4,E4))</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I4" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>177.56</v>
       </c>
       <c r="J4" s="64"/>
     </row>
@@ -3355,7 +3363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding effort for 26.10.2015
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="8" r:id="rId1"/>
@@ -24,12 +24,12 @@
     <definedName name="MemberList">'Team Member'!$B$4:$B$10</definedName>
     <definedName name="SkillList">'Skill Set'!$C$2:$C$34</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="97">
   <si>
     <t>Total</t>
   </si>
@@ -308,16 +308,28 @@
   </si>
   <si>
     <t>Cost Per Anum!</t>
+  </si>
+  <si>
+    <t>26.10.2015</t>
+  </si>
+  <si>
+    <t>Technical Template creation</t>
+  </si>
+  <si>
+    <t>21.10.2015</t>
+  </si>
+  <si>
+    <t>Discussion on how to progress with requirement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1129,6 +1141,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1163,6 +1176,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1338,14 +1352,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:J11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="1"/>
@@ -1353,8 +1365,8 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:15">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -1370,7 +1382,7 @@
       <c r="N2" s="19"/>
       <c r="O2" s="20"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1386,7 +1398,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="21"/>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1402,7 +1414,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="21"/>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1418,7 +1430,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="21"/>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1434,7 +1446,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="21"/>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1450,7 +1462,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="21"/>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1466,7 +1478,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="21"/>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1482,7 +1494,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="21"/>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1500,7 +1512,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="21"/>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1511,7 +1523,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>10239.139000000001</v>
+        <v>11126.929</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1521,7 +1533,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="21"/>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1532,7 +1544,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>28.5</v>
+        <v>30</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1542,7 +1554,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="21"/>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1553,7 +1565,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>3.5625</v>
+        <v>3.75</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1563,7 +1575,7 @@
       <c r="N13" s="4"/>
       <c r="O13" s="21"/>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1579,7 +1591,7 @@
       <c r="N14" s="4"/>
       <c r="O14" s="21"/>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1595,7 +1607,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1611,7 +1623,7 @@
       <c r="N16" s="4"/>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
@@ -1626,7 +1638,7 @@
       <c r="N17" s="4"/>
       <c r="O17" s="21"/>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1641,7 +1653,7 @@
       <c r="N18" s="4"/>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1657,7 +1669,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="2:15" ht="15.75" thickBot="1">
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1690,14 +1702,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
@@ -1719,7 +1731,7 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="84" t="s">
         <v>61</v>
@@ -1742,7 +1754,7 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="11" t="s">
         <v>6</v>
@@ -1773,18 +1785,18 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="14">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>14.5</v>
+        <v>16</v>
       </c>
       <c r="D3" s="33">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>7220.6549999999997</v>
+        <v>8108.4449999999997</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
@@ -1792,11 +1804,11 @@
       </c>
       <c r="G3" s="14">
         <f>SUM(Business!D:D)</f>
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="H3" s="33">
         <f>SUM(Business!I:I)</f>
-        <v>2367.4050000000002</v>
+        <v>2959.2650000000003</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="4"/>
@@ -1808,7 +1820,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="10" t="s">
         <v>10</v>
@@ -1827,11 +1839,11 @@
       </c>
       <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
-        <v>1361.28</v>
+        <v>1657.21</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -1843,7 +1855,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
@@ -1878,7 +1890,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="10" t="s">
         <v>11</v>
@@ -1913,7 +1925,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="10" t="s">
         <v>12</v>
@@ -1948,7 +1960,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="10" t="s">
         <v>13</v>
@@ -1967,11 +1979,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>28.5</v>
+        <v>30</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>10239.139000000001</v>
+        <v>11126.929</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -1983,7 +1995,7 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="10" t="s">
         <v>14</v>
@@ -2010,18 +2022,18 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>28.5</v>
+        <v>30</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>10239.139000000001</v>
+        <v>11126.929</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2037,7 +2049,7 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="16"/>
@@ -2053,7 +2065,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="16"/>
@@ -2069,7 +2081,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="16"/>
@@ -2088,7 +2100,7 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="16"/>
@@ -2107,7 +2119,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="16"/>
@@ -2126,7 +2138,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="16"/>
@@ -2145,7 +2157,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="16"/>
@@ -2164,7 +2176,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="16"/>
@@ -2198,14 +2210,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -2220,7 +2230,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>4</v>
       </c>
@@ -2252,7 +2262,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>51</v>
       </c>
@@ -2289,7 +2299,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>88</v>
       </c>
@@ -2326,22 +2336,30 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="72"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="72">
+        <v>1</v>
+      </c>
       <c r="E4" s="61">
         <f>IF(ISERROR(MATCH(C4,SkillList,0)),0,MATCH(C4,SkillList,0))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F4" s="61">
         <f>IF(ISERROR(MATCH(B4,MemberList,0)),0,MATCH(B4,MemberList,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="62">
         <f>INDEX(CostPerHour,E4)</f>
-        <v>946.97</v>
+        <v>591.86</v>
       </c>
       <c r="H4" s="63">
         <f>IF(ISERROR(INDEX(Competency,F4,E4)), 0, INDEX(Competency,F4,E4))</f>
@@ -2349,11 +2367,13 @@
       </c>
       <c r="I4" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="64"/>
-    </row>
-    <row r="5" spans="1:10">
+        <v>591.86</v>
+      </c>
+      <c r="J4" s="64" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -2380,7 +2400,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -2422,14 +2442,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -2444,7 +2464,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -2476,9 +2496,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="58">
-        <v>42298</v>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>95</v>
       </c>
       <c r="B2" s="59" t="s">
         <v>14</v>
@@ -2511,9 +2531,9 @@
       </c>
       <c r="J2" s="64"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="58">
-        <v>42299</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>75</v>
       </c>
       <c r="B3" s="59" t="s">
         <v>14</v>
@@ -2546,9 +2566,9 @@
       </c>
       <c r="J3" s="64"/>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="58">
-        <v>42301</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>86</v>
       </c>
       <c r="B4" s="59" t="s">
         <v>14</v>
@@ -2581,34 +2601,44 @@
       </c>
       <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="60">
+        <v>0.5</v>
+      </c>
       <c r="E5" s="61">
         <f>IF(ISERROR(MATCH(C5,SkillList,0)),0,MATCH(C5,SkillList,0))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F5" s="61">
         <f>IF(ISERROR(MATCH(B5,MemberList,0)),0,MATCH(B5,MemberList,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="62">
         <f>INDEX(CostPerHour,E5)</f>
-        <v>355.11</v>
+        <v>591.86</v>
       </c>
       <c r="H5" s="63">
         <f>IF(ISERROR(INDEX(Competency,F5,E5)), 0, INDEX(Competency,F5,E5))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I5" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="64"/>
-    </row>
-    <row r="6" spans="1:10">
+        <v>295.93</v>
+      </c>
+      <c r="J5" s="64" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -2649,14 +2679,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -2671,7 +2701,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -2703,7 +2733,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58"/>
       <c r="B2" s="59" t="s">
         <v>8</v>
@@ -2713,19 +2743,19 @@
       </c>
       <c r="D2" s="60"/>
       <c r="E2" s="61">
-        <f>IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
+        <f t="shared" ref="E2:E7" si="0">IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
         <v>8</v>
       </c>
       <c r="F2" s="61">
-        <f>IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
+        <f t="shared" ref="F2:F7" si="1">IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
         <v>3</v>
       </c>
       <c r="G2" s="62">
-        <f>INDEX(CostPerHour,E2)</f>
+        <f t="shared" ref="G2:G7" si="2">INDEX(CostPerHour,E2)</f>
         <v>236.74</v>
       </c>
       <c r="H2" s="63">
-        <f>IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
+        <f t="shared" ref="H2:H7" si="3">IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
         <v>0</v>
       </c>
       <c r="I2" s="62">
@@ -2734,7 +2764,7 @@
       </c>
       <c r="J2" s="64"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58"/>
       <c r="B3" s="59" t="s">
         <v>8</v>
@@ -2744,28 +2774,28 @@
       </c>
       <c r="D3" s="60"/>
       <c r="E3" s="61">
-        <f>IF(ISERROR(MATCH(C3,SkillList,0)),0,MATCH(C3,SkillList,0))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F3" s="61">
-        <f>IF(ISERROR(MATCH(B3,MemberList,0)),0,MATCH(B3,MemberList,0))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G3" s="62">
-        <f>INDEX(CostPerHour,E3)</f>
+        <f t="shared" si="2"/>
         <v>236.74</v>
       </c>
       <c r="H3" s="63">
-        <f>IF(ISERROR(INDEX(Competency,F3,E3)), 0, INDEX(Competency,F3,E3))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I3" s="62">
-        <f t="shared" ref="I3:I5" si="0">D3*G3*H3</f>
+        <f t="shared" ref="I3:I5" si="4">D3*G3*H3</f>
         <v>0</v>
       </c>
       <c r="J3" s="64"/>
     </row>
-    <row r="4" spans="1:10" ht="30">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>75</v>
       </c>
@@ -2779,30 +2809,30 @@
         <v>4</v>
       </c>
       <c r="E4" s="61">
-        <f>IF(ISERROR(MATCH(C4,SkillList,0)),0,MATCH(C4,SkillList,0))</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F4" s="61">
-        <f>IF(ISERROR(MATCH(B4,MemberList,0)),0,MATCH(B4,MemberList,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G4" s="62">
-        <f>INDEX(CostPerHour,E4)</f>
+        <f t="shared" si="2"/>
         <v>591.86</v>
       </c>
       <c r="H4" s="63">
-        <f>IF(ISERROR(INDEX(Competency,F4,E4)), 0, INDEX(Competency,F4,E4))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I4" s="62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2367.44</v>
       </c>
       <c r="J4" s="64" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>75</v>
       </c>
@@ -2816,30 +2846,30 @@
         <v>4</v>
       </c>
       <c r="E5" s="61">
-        <f>IF(ISERROR(MATCH(C5,SkillList,0)),0,MATCH(C5,SkillList,0))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F5" s="61">
-        <f>IF(ISERROR(MATCH(B5,MemberList,0)),0,MATCH(B5,MemberList,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G5" s="62">
-        <f>INDEX(CostPerHour,E5)</f>
+        <f t="shared" si="2"/>
         <v>236.74</v>
       </c>
       <c r="H5" s="63">
-        <f>IF(ISERROR(INDEX(Competency,F5,E5)), 0, INDEX(Competency,F5,E5))</f>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I5" s="62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>189.39200000000002</v>
       </c>
       <c r="J5" s="64" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>86</v>
       </c>
@@ -2853,30 +2883,30 @@
         <v>1</v>
       </c>
       <c r="E6" s="61">
-        <f>IF(ISERROR(MATCH(C6,SkillList,0)),0,MATCH(C6,SkillList,0))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F6" s="61">
-        <f>IF(ISERROR(MATCH(B6,MemberList,0)),0,MATCH(B6,MemberList,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G6" s="62">
-        <f>INDEX(CostPerHour,E6)</f>
+        <f t="shared" si="2"/>
         <v>236.74</v>
       </c>
       <c r="H6" s="63">
-        <f>IF(ISERROR(INDEX(Competency,F6,E6)), 0, INDEX(Competency,F6,E6))</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="I6" s="62">
-        <f t="shared" ref="I6:I7" si="1">D6*G6*H6</f>
+        <f t="shared" ref="I6:I7" si="5">D6*G6*H6</f>
         <v>118.37</v>
       </c>
       <c r="J6" s="64" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>86</v>
       </c>
@@ -2890,30 +2920,30 @@
         <v>1</v>
       </c>
       <c r="E7" s="61">
-        <f>IF(ISERROR(MATCH(C7,SkillList,0)),0,MATCH(C7,SkillList,0))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F7" s="61">
-        <f>IF(ISERROR(MATCH(B7,MemberList,0)),0,MATCH(B7,MemberList,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G7" s="62">
-        <f>INDEX(CostPerHour,E7)</f>
+        <f t="shared" si="2"/>
         <v>236.74</v>
       </c>
       <c r="H7" s="63">
-        <f>IF(ISERROR(INDEX(Competency,F7,E7)), 0, INDEX(Competency,F7,E7))</f>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I7" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>47.348000000000006</v>
       </c>
       <c r="J7" s="64" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="58"/>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -2939,14 +2969,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -2961,7 +2991,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -2993,7 +3023,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>75</v>
       </c>
@@ -3030,7 +3060,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>75</v>
       </c>
@@ -3067,7 +3097,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>75</v>
       </c>
@@ -3104,7 +3134,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -3131,7 +3161,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -3172,14 +3202,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -3194,7 +3224,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -3226,7 +3256,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>84</v>
       </c>
@@ -3263,7 +3293,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58"/>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -3290,7 +3320,7 @@
       </c>
       <c r="J3" s="64"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -3317,7 +3347,7 @@
       </c>
       <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -3344,7 +3374,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -3385,14 +3415,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:AI5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -3405,7 +3435,7 @@
     <col min="30" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="91" t="s">
         <v>81</v>
       </c>
@@ -3446,7 +3476,7 @@
       <c r="AH1" s="89"/>
       <c r="AI1" s="90"/>
     </row>
-    <row r="2" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="92"/>
       <c r="B2" s="92"/>
       <c r="C2" s="93" t="s">
@@ -3493,7 +3523,7 @@
       <c r="AH2" s="86"/>
       <c r="AI2" s="87"/>
     </row>
-    <row r="3" spans="1:35" ht="180">
+    <row r="3" spans="1:35" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
@@ -3600,7 +3630,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
         <v>1</v>
       </c>
@@ -3707,7 +3737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
         <v>2</v>
       </c>
@@ -3814,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="23">
         <v>3</v>
       </c>
@@ -3855,7 +3885,7 @@
       <c r="AH6" s="35"/>
       <c r="AI6" s="44"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>4</v>
       </c>
@@ -3896,7 +3926,7 @@
       <c r="AH7" s="35"/>
       <c r="AI7" s="44"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
         <v>5</v>
       </c>
@@ -3937,7 +3967,7 @@
       <c r="AH8" s="35"/>
       <c r="AI8" s="44"/>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
         <v>6</v>
       </c>
@@ -3978,7 +4008,7 @@
       <c r="AH9" s="35"/>
       <c r="AI9" s="44"/>
     </row>
-    <row r="10" spans="1:35" ht="15.75" thickBot="1">
+    <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>7</v>
       </c>
@@ -4101,12 +4131,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -4116,7 +4146,7 @@
     <col min="7" max="7" width="13.140625" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>69</v>
       </c>
@@ -4139,7 +4169,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="99" t="s">
         <v>25</v>
       </c>
@@ -4166,7 +4196,7 @@
       </c>
       <c r="H2" s="73"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="100"/>
       <c r="B3" s="9">
         <v>2</v>
@@ -4191,7 +4221,7 @@
       </c>
       <c r="H3" s="73"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="100"/>
       <c r="B4" s="9">
         <v>3</v>
@@ -4216,7 +4246,7 @@
       </c>
       <c r="H4" s="73"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="100"/>
       <c r="B5" s="9">
         <v>4</v>
@@ -4241,7 +4271,7 @@
       </c>
       <c r="H5" s="73"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="100"/>
       <c r="B6" s="9">
         <v>5</v>
@@ -4266,7 +4296,7 @@
       </c>
       <c r="H6" s="73"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="101"/>
       <c r="B7" s="9">
         <v>6</v>
@@ -4291,7 +4321,7 @@
       </c>
       <c r="H7" s="73"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="99" t="s">
         <v>29</v>
       </c>
@@ -4317,7 +4347,7 @@
         <v>591.86</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="100"/>
       <c r="B9" s="9">
         <v>8</v>
@@ -4341,7 +4371,7 @@
         <v>236.74</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
       <c r="B10" s="9">
         <v>9</v>
@@ -4365,7 +4395,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="100"/>
       <c r="B11" s="9">
         <v>10</v>
@@ -4389,7 +4419,7 @@
         <v>591.86</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="100"/>
       <c r="B12" s="9">
         <v>11</v>
@@ -4413,7 +4443,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="100"/>
       <c r="B13" s="9">
         <v>12</v>
@@ -4437,7 +4467,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="100"/>
       <c r="B14" s="9">
         <v>13</v>
@@ -4461,7 +4491,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="100"/>
       <c r="B15" s="9">
         <v>14</v>
@@ -4485,7 +4515,7 @@
         <v>295.93</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="100"/>
       <c r="B16" s="9">
         <v>15</v>
@@ -4509,7 +4539,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="99" t="s">
         <v>67</v>
       </c>
@@ -4535,7 +4565,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="100"/>
       <c r="B18" s="9">
         <v>17</v>
@@ -4559,7 +4589,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
       <c r="B19" s="9">
         <v>18</v>
@@ -4583,7 +4613,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="100"/>
       <c r="B20" s="9">
         <v>19</v>
@@ -4607,7 +4637,7 @@
         <v>236.74</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="100"/>
       <c r="B21" s="9">
         <v>20</v>
@@ -4631,7 +4661,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="100"/>
       <c r="B22" s="9">
         <v>21</v>
@@ -4655,7 +4685,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="100"/>
       <c r="B23" s="9">
         <v>22</v>
@@ -4679,7 +4709,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="100"/>
       <c r="B24" s="9">
         <v>23</v>
@@ -4703,7 +4733,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="100"/>
       <c r="B25" s="9">
         <v>24</v>
@@ -4727,7 +4757,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="101"/>
       <c r="B26" s="9">
         <v>25</v>
@@ -4751,7 +4781,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="99" t="s">
         <v>68</v>
       </c>
@@ -4777,7 +4807,7 @@
         <v>295.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="100"/>
       <c r="B28" s="9">
         <v>27</v>
@@ -4801,7 +4831,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="100"/>
       <c r="B29" s="9">
         <v>28</v>
@@ -4825,7 +4855,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="101"/>
       <c r="B30" s="9">
         <v>29</v>
@@ -4849,7 +4879,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="99" t="s">
         <v>28</v>
       </c>
@@ -4875,7 +4905,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="100"/>
       <c r="B32" s="9">
         <v>31</v>
@@ -4899,7 +4929,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="100"/>
       <c r="B33" s="9">
         <v>32</v>
@@ -4923,7 +4953,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="100"/>
       <c r="B34" s="9">
         <v>33</v>

</xml_diff>

<commit_message>
Changing model by introducing iterative approach for requirement
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785"/>
+    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="8" r:id="rId1"/>
@@ -319,7 +319,7 @@
     <t>21.10.2015</t>
   </si>
   <si>
-    <t>Discussion on how to progress with requirement</t>
+    <t>Discussion on how to progress with requirement, Changing model</t>
   </si>
 </sst>
 </file>
@@ -1355,7 +1355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1523,7 +1523,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>11126.929</v>
+        <v>11422.859</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1544,7 +1544,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>30</v>
+        <v>30.5</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1565,7 +1565,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>3.75</v>
+        <v>3.8125</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1792,11 +1792,11 @@
       </c>
       <c r="C3" s="14">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>16</v>
+        <v>16.5</v>
       </c>
       <c r="D3" s="33">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>8108.4449999999997</v>
+        <v>8404.375</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
@@ -1839,11 +1839,11 @@
       </c>
       <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
-        <v>1657.21</v>
+        <v>1953.1399999999999</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -1979,11 +1979,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>30</v>
+        <v>30.5</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>11126.929</v>
+        <v>11422.859</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -2029,11 +2029,11 @@
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>30</v>
+        <v>30.5</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>11126.929</v>
+        <v>11422.859</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2445,8 +2445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2612,7 +2612,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="60">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E5" s="61">
         <f>IF(ISERROR(MATCH(C5,SkillList,0)),0,MATCH(C5,SkillList,0))</f>
@@ -2632,7 +2632,7 @@
       </c>
       <c r="I5" s="62">
         <f t="shared" si="0"/>
-        <v>295.93</v>
+        <v>591.86</v>
       </c>
       <c r="J5" s="64" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Adding business analysis for School
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="99">
   <si>
     <t>Total</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t>Discussion on how to progress with requirement, Changing model</t>
+  </si>
+  <si>
+    <t>27.10.2015</t>
+  </si>
+  <si>
+    <t>Adding requirement using use case and class diagram</t>
   </si>
 </sst>
 </file>
@@ -1523,7 +1529,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>11422.859</v>
+        <v>11600.419000000002</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1544,7 +1550,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>30.5</v>
+        <v>31.5</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1565,7 +1571,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>3.8125</v>
+        <v>3.9375</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1792,11 +1798,11 @@
       </c>
       <c r="C3" s="14">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
       <c r="D3" s="33">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>8404.375</v>
+        <v>8581.9350000000013</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
@@ -1839,11 +1845,11 @@
       </c>
       <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
-        <v>1953.1399999999999</v>
+        <v>2130.6999999999998</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -1979,11 +1985,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>30.5</v>
+        <v>31.5</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>11422.859</v>
+        <v>11600.419</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -2029,11 +2035,11 @@
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>30.5</v>
+        <v>31.5</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>11422.859</v>
+        <v>11600.419000000002</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2213,7 +2219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2443,10 +2451,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2561,7 +2569,7 @@
         <v>0.5</v>
       </c>
       <c r="I3" s="62">
-        <f t="shared" ref="I3:I6" si="0">D3*G3*H3</f>
+        <f t="shared" ref="I3:I5" si="0">D3*G3*H3</f>
         <v>591.86</v>
       </c>
       <c r="J3" s="64"/>
@@ -2639,31 +2647,101 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60"/>
+      <c r="A6" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="60">
+        <v>1</v>
+      </c>
       <c r="E6" s="61">
         <f>IF(ISERROR(MATCH(C6,SkillList,0)),0,MATCH(C6,SkillList,0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F6" s="61">
         <f>IF(ISERROR(MATCH(B6,MemberList,0)),0,MATCH(B6,MemberList,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="62">
         <f>INDEX(CostPerHour,E6)</f>
-        <v>355.11</v>
+        <v>177.56</v>
       </c>
       <c r="H6" s="63">
         <f>IF(ISERROR(INDEX(Competency,F6,E6)), 0, INDEX(Competency,F6,E6))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="64"/>
+        <f t="shared" ref="I6" si="1">D6*G6*H6</f>
+        <v>177.56</v>
+      </c>
+      <c r="J6" s="64" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="58"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="64"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="64"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="58"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="64"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="64"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="58"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="64"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Adding effort in business modelling for Retinue
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="8" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="101">
   <si>
     <t>Total</t>
   </si>
@@ -326,6 +326,12 @@
   </si>
   <si>
     <t>Adding requirement using use case and class diagram</t>
+  </si>
+  <si>
+    <t>27.10.2016</t>
+  </si>
+  <si>
+    <t>Calculating sales commision, and how it will fit</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1529,7 +1535,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>11600.419000000002</v>
+        <v>11896.349</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1550,7 +1556,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>31.5</v>
+        <v>32</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1571,7 +1577,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>3.9375</v>
+        <v>4</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1798,11 +1804,11 @@
       </c>
       <c r="C3" s="14">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>17.5</v>
+        <v>18</v>
       </c>
       <c r="D3" s="33">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>8581.9350000000013</v>
+        <v>8877.8649999999998</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
@@ -1950,11 +1956,11 @@
       </c>
       <c r="G7" s="14">
         <f>SUM(Tourism!D:D)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H7" s="33">
         <f>SUM(Tourism!I:I)</f>
-        <v>1775.58</v>
+        <v>2071.5099999999998</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="4"/>
@@ -1985,11 +1991,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>31.5</v>
+        <v>32</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>11600.419</v>
+        <v>11896.349</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -2035,11 +2041,11 @@
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>31.5</v>
+        <v>32</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>11600.419000000002</v>
+        <v>11896.349</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2453,7 +2459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -3284,7 +3290,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3372,31 +3378,41 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="60"/>
+      <c r="A3" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="60">
+        <v>0.5</v>
+      </c>
       <c r="E3" s="61">
         <f>IF(ISERROR(MATCH(C3,SkillList,0)),0,MATCH(C3,SkillList,0))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F3" s="61">
         <f>IF(ISERROR(MATCH(B3,MemberList,0)),0,MATCH(B3,MemberList,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="62">
         <f>INDEX(CostPerHour,E3)</f>
-        <v>946.97</v>
+        <v>591.86</v>
       </c>
       <c r="H3" s="63">
         <f>IF(ISERROR(INDEX(Competency,F3,E3)), 0, INDEX(Competency,F3,E3))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="62">
         <f t="shared" ref="I3:I6" si="0">D3*G3*H3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="64"/>
+        <v>295.93</v>
+      </c>
+      <c r="J3" s="64" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58"/>

</xml_diff>

<commit_message>
Changing activity diagram for collect fee
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785"/>
+    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="8" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="102">
   <si>
     <t>Total</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>Calculating sales commision, and how it will fit</t>
+  </si>
+  <si>
+    <t>28.10.2015</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1535,7 +1538,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>11896.349</v>
+        <v>12073.909</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1556,7 +1559,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1577,7 +1580,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>4</v>
+        <v>4.125</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1804,11 +1807,11 @@
       </c>
       <c r="C3" s="14">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="33">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>8877.8649999999998</v>
+        <v>9055.4249999999993</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
@@ -1851,11 +1854,11 @@
       </c>
       <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
-        <v>2130.6999999999998</v>
+        <v>2308.2599999999998</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -1991,11 +1994,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>11896.349</v>
+        <v>12073.909</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -2041,11 +2044,11 @@
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>11896.349</v>
+        <v>12073.909</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2459,8 +2462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2682,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="62">
-        <f t="shared" ref="I6" si="1">D6*G6*H6</f>
+        <f t="shared" ref="I6:I11" si="1">D6*G6*H6</f>
         <v>177.56</v>
       </c>
       <c r="J6" s="64" t="s">
@@ -2690,15 +2693,38 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="62"/>
+      <c r="A7" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="60">
+        <v>1</v>
+      </c>
+      <c r="E7" s="61">
+        <f>IF(ISERROR(MATCH(C7,SkillList,0)),0,MATCH(C7,SkillList,0))</f>
+        <v>9</v>
+      </c>
+      <c r="F7" s="61">
+        <f>IF(ISERROR(MATCH(B7,MemberList,0)),0,MATCH(B7,MemberList,0))</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="62">
+        <f>INDEX(CostPerHour,E7)</f>
+        <v>177.56</v>
+      </c>
+      <c r="H7" s="63">
+        <f>IF(ISERROR(INDEX(Competency,F7,E7)), 0, INDEX(Competency,F7,E7))</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="62">
+        <f t="shared" si="1"/>
+        <v>177.56</v>
+      </c>
       <c r="J7" s="64"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2706,11 +2732,26 @@
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
       <c r="D8" s="60"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="62"/>
+      <c r="E8" s="61">
+        <f>IF(ISERROR(MATCH(C8,SkillList,0)),0,MATCH(C8,SkillList,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="61">
+        <f>IF(ISERROR(MATCH(B8,MemberList,0)),0,MATCH(B8,MemberList,0))</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="62">
+        <f>INDEX(CostPerHour,E8)</f>
+        <v>591.86</v>
+      </c>
+      <c r="H8" s="63">
+        <f>IF(ISERROR(INDEX(Competency,F8,E8)), 0, INDEX(Competency,F8,E8))</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J8" s="64"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2718,11 +2759,26 @@
       <c r="B9" s="59"/>
       <c r="C9" s="59"/>
       <c r="D9" s="60"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="62"/>
+      <c r="E9" s="61">
+        <f>IF(ISERROR(MATCH(C9,SkillList,0)),0,MATCH(C9,SkillList,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="61">
+        <f>IF(ISERROR(MATCH(B9,MemberList,0)),0,MATCH(B9,MemberList,0))</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="62">
+        <f>INDEX(CostPerHour,E9)</f>
+        <v>236.74</v>
+      </c>
+      <c r="H9" s="63">
+        <f>IF(ISERROR(INDEX(Competency,F9,E9)), 0, INDEX(Competency,F9,E9))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J9" s="64"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2730,11 +2786,26 @@
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
       <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="62"/>
+      <c r="E10" s="61">
+        <f>IF(ISERROR(MATCH(C10,SkillList,0)),0,MATCH(C10,SkillList,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="61">
+        <f>IF(ISERROR(MATCH(B10,MemberList,0)),0,MATCH(B10,MemberList,0))</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="62">
+        <f>INDEX(CostPerHour,E10)</f>
+        <v>177.56</v>
+      </c>
+      <c r="H10" s="63">
+        <f>IF(ISERROR(INDEX(Competency,F10,E10)), 0, INDEX(Competency,F10,E10))</f>
+        <v>0.25</v>
+      </c>
+      <c r="I10" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J10" s="64"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2742,11 +2813,26 @@
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
       <c r="D11" s="60"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="62"/>
+      <c r="E11" s="61">
+        <f>IF(ISERROR(MATCH(C11,SkillList,0)),0,MATCH(C11,SkillList,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="61">
+        <f>IF(ISERROR(MATCH(B11,MemberList,0)),0,MATCH(B11,MemberList,0))</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="62">
+        <f>INDEX(CostPerHour,E11)</f>
+        <v>591.86</v>
+      </c>
+      <c r="H11" s="63">
+        <f>IF(ISERROR(INDEX(Competency,F11,E11)), 0, INDEX(Competency,F11,E11))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J11" s="64"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding effort for 04.11.2015
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="111">
   <si>
     <t>Total</t>
   </si>
@@ -353,6 +353,15 @@
   </si>
   <si>
     <t>Making model iterative</t>
+  </si>
+  <si>
+    <t>04.11.2015</t>
+  </si>
+  <si>
+    <t>Modeling student</t>
+  </si>
+  <si>
+    <t>Developed basic framework and studen as test form</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +1565,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>14441.329000000002</v>
+        <v>15003.589000000002</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1577,7 +1586,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>45</v>
+        <v>49.5</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1598,7 +1607,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>5.625</v>
+        <v>6.1875</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1825,11 +1834,11 @@
       </c>
       <c r="C3" s="14">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>31</v>
+        <v>35.5</v>
       </c>
       <c r="D3" s="33">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>11422.845000000001</v>
+        <v>11985.105000000001</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
@@ -1872,11 +1881,11 @@
       </c>
       <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
-        <v>21</v>
+        <v>25.5</v>
       </c>
       <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
-        <v>4675.6799999999994</v>
+        <v>5237.9399999999987</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -2012,11 +2021,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>45</v>
+        <v>49.5</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>14441.329</v>
+        <v>15003.588999999998</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -2062,11 +2071,11 @@
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>45</v>
+        <v>49.5</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>14441.329000000002</v>
+        <v>15003.589000000002</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2481,7 +2490,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2859,58 +2868,78 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="60"/>
+      <c r="A11" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="60">
+        <v>0.5</v>
+      </c>
       <c r="E11" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F11" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="62">
         <f t="shared" si="2"/>
-        <v>591.86</v>
+        <v>177.56</v>
       </c>
       <c r="H11" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="64"/>
+        <v>88.78</v>
+      </c>
+      <c r="J11" s="64" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="60"/>
+      <c r="A12" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="60">
+        <v>4</v>
+      </c>
       <c r="E12" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F12" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="62">
         <f t="shared" si="2"/>
-        <v>177.56</v>
+        <v>118.37</v>
       </c>
       <c r="H12" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="64"/>
+        <v>473.48</v>
+      </c>
+      <c r="J12" s="64" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="58"/>

</xml_diff>

<commit_message>
Adding effort for 05.11.2015
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="113">
   <si>
     <t>Total</t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>Developed basic framework and studen as test form</t>
+  </si>
+  <si>
+    <t>05.11.2015</t>
+  </si>
+  <si>
+    <t>Restructuring UI using control. Training for Sample code.</t>
   </si>
 </sst>
 </file>
@@ -1565,7 +1571,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>15003.589000000002</v>
+        <v>15477.069000000001</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1586,7 +1592,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>49.5</v>
+        <v>53.5</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1607,7 +1613,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>6.1875</v>
+        <v>6.6875</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1834,11 +1840,11 @@
       </c>
       <c r="C3" s="14">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>35.5</v>
+        <v>39.5</v>
       </c>
       <c r="D3" s="33">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>11985.105000000001</v>
+        <v>12458.585000000001</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
@@ -1881,11 +1887,11 @@
       </c>
       <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
-        <v>25.5</v>
+        <v>29.5</v>
       </c>
       <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
-        <v>5237.9399999999987</v>
+        <v>5711.4199999999983</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -2021,11 +2027,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>49.5</v>
+        <v>53.5</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>15003.588999999998</v>
+        <v>15477.068999999998</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -2071,11 +2077,11 @@
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>49.5</v>
+        <v>53.5</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>15003.589000000002</v>
+        <v>15477.069000000001</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2490,7 +2496,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2942,17 +2948,25 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="60"/>
+      <c r="A13" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="60">
+        <v>4</v>
+      </c>
       <c r="E13" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F13" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="62">
         <f t="shared" si="2"/>
@@ -2960,13 +2974,15 @@
       </c>
       <c r="H13" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="64"/>
+        <v>473.48</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="58"/>

</xml_diff>

<commit_message>
Working on School project
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="3"/>
@@ -24,12 +24,12 @@
     <definedName name="MemberList">'Team Member'!$B$4:$B$10</definedName>
     <definedName name="SkillList">'Skill Set'!$C$2:$C$34</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="116">
   <si>
     <t>Total</t>
   </si>
@@ -368,16 +368,25 @@
   </si>
   <si>
     <t>Restructuring UI using control. Training for Sample code.</t>
+  </si>
+  <si>
+    <t>Added Gender component</t>
+  </si>
+  <si>
+    <t>Added Religion component</t>
+  </si>
+  <si>
+    <t>06.11.2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1189,7 +1198,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1224,7 +1232,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1400,12 +1407,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="1"/>
@@ -1413,8 +1420,8 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:15">
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -1430,7 +1437,7 @@
       <c r="N2" s="19"/>
       <c r="O2" s="20"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1446,7 +1453,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="21"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15">
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1462,7 +1469,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="21"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1478,7 +1485,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="21"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1494,7 +1501,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="21"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1510,7 +1517,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="21"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15">
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1526,7 +1533,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="21"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1542,7 +1549,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="21"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1560,7 +1567,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="21"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1571,7 +1578,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>15477.069000000001</v>
+        <v>15565.8465</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1581,7 +1588,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="21"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1592,7 +1599,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>53.5</v>
+        <v>56.5</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1602,7 +1609,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="21"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15">
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1613,7 +1620,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>6.6875</v>
+        <v>7.0625</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1623,7 +1630,7 @@
       <c r="N13" s="4"/>
       <c r="O13" s="21"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1639,7 +1646,7 @@
       <c r="N14" s="4"/>
       <c r="O14" s="21"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1655,7 +1662,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15">
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1671,7 +1678,7 @@
       <c r="N16" s="4"/>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15">
       <c r="B17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
@@ -1686,7 +1693,7 @@
       <c r="N17" s="4"/>
       <c r="O17" s="21"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1701,7 +1708,7 @@
       <c r="N18" s="4"/>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1717,7 +1724,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:15" ht="15.75" thickBot="1">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1750,14 +1757,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
@@ -1779,7 +1786,7 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="4"/>
       <c r="B1" s="84" t="s">
         <v>61</v>
@@ -1802,7 +1809,7 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="4"/>
       <c r="B2" s="11" t="s">
         <v>6</v>
@@ -1833,7 +1840,7 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="4"/>
       <c r="B3" s="10" t="s">
         <v>7</v>
@@ -1868,7 +1875,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="4"/>
       <c r="B4" s="10" t="s">
         <v>10</v>
@@ -1887,11 +1894,11 @@
       </c>
       <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
-        <v>29.5</v>
+        <v>32.5</v>
       </c>
       <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
-        <v>5711.4199999999983</v>
+        <v>5800.1974999999984</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -1903,7 +1910,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="4"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
@@ -1938,7 +1945,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="4"/>
       <c r="B6" s="10" t="s">
         <v>11</v>
@@ -1973,7 +1980,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="4"/>
       <c r="B7" s="10" t="s">
         <v>12</v>
@@ -2008,7 +2015,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="4"/>
       <c r="B8" s="10" t="s">
         <v>13</v>
@@ -2027,11 +2034,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>53.5</v>
+        <v>56.5</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>15477.068999999998</v>
+        <v>15565.846499999998</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -2043,18 +2050,18 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="4"/>
       <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="14">
         <f>SUMIF(Business!B:B,B9,Business!D:D) + SUMIF(School!B:B,B9,School!D:D) + SUMIF(Service!B:B,B9,Service!D:D)+SUMIF(Retail!B:B,B9,Retail!D:D) + SUMIF(Tourism!B:B,B9,Tourism!D:D)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D9" s="33">
         <f>SUMIF(Business!B:B,B9,Business!I:I) + SUMIF(School!B:B,B9,School!I:I) + SUMIF(Service!B:B,B9,Service!I:I)+SUMIF(Retail!B:B,B9,Retail!I:I) + SUMIF(Tourism!B:B,B9,Tourism!I:I)</f>
-        <v>1361.28</v>
+        <v>1450.0574999999999</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
@@ -2070,18 +2077,18 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" s="4"/>
       <c r="B10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>53.5</v>
+        <v>56.5</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>15477.069000000001</v>
+        <v>15565.8465</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2097,7 +2104,7 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="16"/>
@@ -2113,7 +2120,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="16"/>
@@ -2129,7 +2136,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="16"/>
@@ -2148,7 +2155,7 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="16"/>
@@ -2167,7 +2174,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="16"/>
@@ -2186,7 +2193,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="16"/>
@@ -2205,7 +2212,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="16"/>
@@ -2224,7 +2231,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="16"/>
@@ -2258,14 +2265,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -2280,7 +2287,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="69" t="s">
         <v>4</v>
       </c>
@@ -2312,7 +2319,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="58" t="s">
         <v>51</v>
       </c>
@@ -2349,7 +2356,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="58" t="s">
         <v>88</v>
       </c>
@@ -2386,7 +2393,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="58" t="s">
         <v>93</v>
       </c>
@@ -2423,7 +2430,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -2450,7 +2457,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -2492,14 +2499,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -2514,7 +2521,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -2546,7 +2553,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="58" t="s">
         <v>95</v>
       </c>
@@ -2581,7 +2588,7 @@
       </c>
       <c r="J2" s="64"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="58" t="s">
         <v>75</v>
       </c>
@@ -2616,7 +2623,7 @@
       </c>
       <c r="J3" s="64"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="58" t="s">
         <v>86</v>
       </c>
@@ -2651,7 +2658,7 @@
       </c>
       <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="58" t="s">
         <v>93</v>
       </c>
@@ -2688,7 +2695,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="58" t="s">
         <v>97</v>
       </c>
@@ -2725,7 +2732,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="58" t="s">
         <v>101</v>
       </c>
@@ -2762,7 +2769,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="58" t="s">
         <v>102</v>
       </c>
@@ -2799,7 +2806,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="58" t="s">
         <v>102</v>
       </c>
@@ -2836,7 +2843,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="58" t="s">
         <v>103</v>
       </c>
@@ -2873,7 +2880,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="58" t="s">
         <v>108</v>
       </c>
@@ -2910,7 +2917,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="58" t="s">
         <v>108</v>
       </c>
@@ -2947,7 +2954,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="58" t="s">
         <v>111</v>
       </c>
@@ -2984,18 +2991,26 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="60"/>
+    <row r="14" spans="1:10">
+      <c r="A14" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="60">
+        <v>2</v>
+      </c>
       <c r="E14" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F14" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G14" s="62">
         <f t="shared" si="2"/>
@@ -3003,42 +3018,54 @@
       </c>
       <c r="H14" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I14" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="64"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60"/>
+        <v>59.185000000000002</v>
+      </c>
+      <c r="J14" s="64" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="60">
+        <v>1</v>
+      </c>
       <c r="E15" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F15" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G15" s="62">
         <f t="shared" si="2"/>
-        <v>295.93</v>
+        <v>118.37</v>
       </c>
       <c r="H15" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I15" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="64"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>29.592500000000001</v>
+      </c>
+      <c r="J15" s="64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="58"/>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
@@ -3065,7 +3092,7 @@
       </c>
       <c r="J16" s="64"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="58"/>
       <c r="B17" s="59"/>
       <c r="C17" s="59"/>
@@ -3092,7 +3119,7 @@
       </c>
       <c r="J17" s="64"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="58"/>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
@@ -3119,7 +3146,7 @@
       </c>
       <c r="J18" s="64"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="58"/>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
@@ -3160,14 +3187,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -3182,7 +3209,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -3214,7 +3241,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="58"/>
       <c r="B2" s="59" t="s">
         <v>8</v>
@@ -3245,7 +3272,7 @@
       </c>
       <c r="J2" s="64"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="58"/>
       <c r="B3" s="59" t="s">
         <v>8</v>
@@ -3276,7 +3303,7 @@
       </c>
       <c r="J3" s="64"/>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30">
       <c r="A4" s="58" t="s">
         <v>75</v>
       </c>
@@ -3313,7 +3340,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="58" t="s">
         <v>75</v>
       </c>
@@ -3350,7 +3377,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="58" t="s">
         <v>86</v>
       </c>
@@ -3387,7 +3414,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="58" t="s">
         <v>86</v>
       </c>
@@ -3424,7 +3451,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="58"/>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -3450,14 +3477,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -3472,7 +3499,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -3504,7 +3531,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="58" t="s">
         <v>75</v>
       </c>
@@ -3541,7 +3568,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="58" t="s">
         <v>75</v>
       </c>
@@ -3578,7 +3605,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="58" t="s">
         <v>75</v>
       </c>
@@ -3615,7 +3642,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -3642,7 +3669,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -3683,14 +3710,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -3705,7 +3732,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -3737,7 +3764,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="58" t="s">
         <v>84</v>
       </c>
@@ -3774,7 +3801,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="58" t="s">
         <v>99</v>
       </c>
@@ -3811,7 +3838,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="58"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -3838,7 +3865,7 @@
       </c>
       <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -3865,7 +3892,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -3906,14 +3933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -3926,7 +3953,7 @@
     <col min="30" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="91" t="s">
         <v>81</v>
       </c>
@@ -3967,7 +3994,7 @@
       <c r="AH1" s="89"/>
       <c r="AI1" s="90"/>
     </row>
-    <row r="2" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="92"/>
       <c r="B2" s="92"/>
       <c r="C2" s="93" t="s">
@@ -4014,7 +4041,7 @@
       <c r="AH2" s="86"/>
       <c r="AI2" s="87"/>
     </row>
-    <row r="3" spans="1:35" ht="180" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="180">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
@@ -4121,7 +4148,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35">
       <c r="A4" s="23">
         <v>1</v>
       </c>
@@ -4228,7 +4255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35">
       <c r="A5" s="23">
         <v>2</v>
       </c>
@@ -4335,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35">
       <c r="A6" s="23">
         <v>3</v>
       </c>
@@ -4376,7 +4403,7 @@
       <c r="AH6" s="35"/>
       <c r="AI6" s="44"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35">
       <c r="A7" s="23">
         <v>4</v>
       </c>
@@ -4417,7 +4444,7 @@
       <c r="AH7" s="35"/>
       <c r="AI7" s="44"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35">
       <c r="A8" s="23">
         <v>5</v>
       </c>
@@ -4458,7 +4485,7 @@
       <c r="AH8" s="35"/>
       <c r="AI8" s="44"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35">
       <c r="A9" s="23">
         <v>6</v>
       </c>
@@ -4499,7 +4526,7 @@
       <c r="AH9" s="35"/>
       <c r="AI9" s="44"/>
     </row>
-    <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" ht="15.75" thickBot="1">
       <c r="A10" s="23">
         <v>7</v>
       </c>
@@ -4540,7 +4567,7 @@
         <v>0.25</v>
       </c>
       <c r="N10" s="47">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="O10" s="47">
         <v>0.5</v>
@@ -4622,12 +4649,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -4637,7 +4664,7 @@
     <col min="7" max="7" width="13.140625" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="11" t="s">
         <v>69</v>
       </c>
@@ -4660,7 +4687,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="99" t="s">
         <v>25</v>
       </c>
@@ -4687,7 +4714,7 @@
       </c>
       <c r="H2" s="73"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="100"/>
       <c r="B3" s="9">
         <v>2</v>
@@ -4712,7 +4739,7 @@
       </c>
       <c r="H3" s="73"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="100"/>
       <c r="B4" s="9">
         <v>3</v>
@@ -4737,7 +4764,7 @@
       </c>
       <c r="H4" s="73"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="100"/>
       <c r="B5" s="9">
         <v>4</v>
@@ -4762,7 +4789,7 @@
       </c>
       <c r="H5" s="73"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="100"/>
       <c r="B6" s="9">
         <v>5</v>
@@ -4787,7 +4814,7 @@
       </c>
       <c r="H6" s="73"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="101"/>
       <c r="B7" s="9">
         <v>6</v>
@@ -4812,7 +4839,7 @@
       </c>
       <c r="H7" s="73"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="99" t="s">
         <v>29</v>
       </c>
@@ -4838,7 +4865,7 @@
         <v>591.86</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="100"/>
       <c r="B9" s="9">
         <v>8</v>
@@ -4862,7 +4889,7 @@
         <v>236.74</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="100"/>
       <c r="B10" s="9">
         <v>9</v>
@@ -4886,7 +4913,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="100"/>
       <c r="B11" s="9">
         <v>10</v>
@@ -4910,7 +4937,7 @@
         <v>591.86</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="100"/>
       <c r="B12" s="9">
         <v>11</v>
@@ -4934,7 +4961,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="100"/>
       <c r="B13" s="9">
         <v>12</v>
@@ -4958,7 +4985,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="100"/>
       <c r="B14" s="9">
         <v>13</v>
@@ -4982,7 +5009,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="100"/>
       <c r="B15" s="9">
         <v>14</v>
@@ -5006,7 +5033,7 @@
         <v>295.93</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="100"/>
       <c r="B16" s="9">
         <v>15</v>
@@ -5030,7 +5057,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="99" t="s">
         <v>67</v>
       </c>
@@ -5056,7 +5083,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="100"/>
       <c r="B18" s="9">
         <v>17</v>
@@ -5080,7 +5107,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="100"/>
       <c r="B19" s="9">
         <v>18</v>
@@ -5104,7 +5131,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="100"/>
       <c r="B20" s="9">
         <v>19</v>
@@ -5128,7 +5155,7 @@
         <v>236.74</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="100"/>
       <c r="B21" s="9">
         <v>20</v>
@@ -5152,7 +5179,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="100"/>
       <c r="B22" s="9">
         <v>21</v>
@@ -5176,7 +5203,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="100"/>
       <c r="B23" s="9">
         <v>22</v>
@@ -5200,7 +5227,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="100"/>
       <c r="B24" s="9">
         <v>23</v>
@@ -5224,7 +5251,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="100"/>
       <c r="B25" s="9">
         <v>24</v>
@@ -5248,7 +5275,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="101"/>
       <c r="B26" s="9">
         <v>25</v>
@@ -5272,7 +5299,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="99" t="s">
         <v>68</v>
       </c>
@@ -5298,7 +5325,7 @@
         <v>295.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="100"/>
       <c r="B28" s="9">
         <v>27</v>
@@ -5322,7 +5349,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="100"/>
       <c r="B29" s="9">
         <v>28</v>
@@ -5346,7 +5373,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="101"/>
       <c r="B30" s="9">
         <v>29</v>
@@ -5370,7 +5397,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="99" t="s">
         <v>28</v>
       </c>
@@ -5396,7 +5423,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="100"/>
       <c r="B32" s="9">
         <v>31</v>
@@ -5420,7 +5447,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="100"/>
       <c r="B33" s="9">
         <v>32</v>
@@ -5444,7 +5471,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="100"/>
       <c r="B34" s="9">
         <v>33</v>

</xml_diff>

<commit_message>
Adding effort for 7th and 10th Nov
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="3"/>
@@ -24,12 +24,12 @@
     <definedName name="MemberList">'Team Member'!$B$4:$B$10</definedName>
     <definedName name="SkillList">'Skill Set'!$C$2:$C$34</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="120">
   <si>
     <t>Total</t>
   </si>
@@ -377,16 +377,28 @@
   </si>
   <si>
     <t>06.11.2015</t>
+  </si>
+  <si>
+    <t>07.11.2015</t>
+  </si>
+  <si>
+    <t>Wireframe for student</t>
+  </si>
+  <si>
+    <t>10.11.2015</t>
+  </si>
+  <si>
+    <t>Billing design, discussion for fees</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1198,6 +1210,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1232,6 +1245,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1407,12 +1421,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="1"/>
@@ -1420,8 +1434,8 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:15">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -1437,7 +1451,7 @@
       <c r="N2" s="19"/>
       <c r="O2" s="20"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1453,7 +1467,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="21"/>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1469,7 +1483,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="21"/>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1485,7 +1499,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="21"/>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1501,7 +1515,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="21"/>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1517,7 +1531,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="21"/>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1533,7 +1547,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="21"/>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1549,7 +1563,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="21"/>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1567,7 +1581,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="21"/>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1578,7 +1592,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>15565.8465</v>
+        <v>16335.266500000002</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1588,7 +1602,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="21"/>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1599,7 +1613,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>56.5</v>
+        <v>61.5</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1609,7 +1623,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="21"/>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1620,7 +1634,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>7.0625</v>
+        <v>7.6875</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1630,7 +1644,7 @@
       <c r="N13" s="4"/>
       <c r="O13" s="21"/>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1646,7 +1660,7 @@
       <c r="N14" s="4"/>
       <c r="O14" s="21"/>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1662,7 +1676,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1678,7 +1692,7 @@
       <c r="N16" s="4"/>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
@@ -1693,7 +1707,7 @@
       <c r="N17" s="4"/>
       <c r="O17" s="21"/>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1708,7 +1722,7 @@
       <c r="N18" s="4"/>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1724,7 +1738,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="2:15" ht="15.75" thickBot="1">
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1757,14 +1771,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
@@ -1786,7 +1800,7 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="84" t="s">
         <v>61</v>
@@ -1809,7 +1823,7 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="11" t="s">
         <v>6</v>
@@ -1840,18 +1854,18 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="14">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>39.5</v>
+        <v>44.5</v>
       </c>
       <c r="D3" s="33">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>12458.585000000001</v>
+        <v>13228.005000000001</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
@@ -1875,7 +1889,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="10" t="s">
         <v>10</v>
@@ -1894,11 +1908,11 @@
       </c>
       <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
-        <v>32.5</v>
+        <v>37.5</v>
       </c>
       <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
-        <v>5800.1974999999984</v>
+        <v>6569.6174999999985</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -1910,7 +1924,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
@@ -1945,7 +1959,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="10" t="s">
         <v>11</v>
@@ -1980,7 +1994,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="10" t="s">
         <v>12</v>
@@ -2015,7 +2029,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="10" t="s">
         <v>13</v>
@@ -2034,11 +2048,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>56.5</v>
+        <v>61.5</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>15565.846499999998</v>
+        <v>16335.2665</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -2050,7 +2064,7 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="10" t="s">
         <v>14</v>
@@ -2077,18 +2091,18 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>56.5</v>
+        <v>61.5</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>15565.8465</v>
+        <v>16335.266500000002</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2104,7 +2118,7 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="16"/>
@@ -2120,7 +2134,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="16"/>
@@ -2136,7 +2150,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="16"/>
@@ -2155,7 +2169,7 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="16"/>
@@ -2174,7 +2188,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="16"/>
@@ -2193,7 +2207,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="16"/>
@@ -2212,7 +2226,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="16"/>
@@ -2231,7 +2245,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="16"/>
@@ -2265,14 +2279,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -2287,7 +2301,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>4</v>
       </c>
@@ -2319,7 +2333,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>51</v>
       </c>
@@ -2356,7 +2370,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>88</v>
       </c>
@@ -2393,7 +2407,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>93</v>
       </c>
@@ -2430,7 +2444,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -2457,7 +2471,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -2499,14 +2513,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -2521,7 +2535,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -2553,7 +2567,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>95</v>
       </c>
@@ -2567,19 +2581,19 @@
         <v>2</v>
       </c>
       <c r="E2" s="61">
-        <f t="shared" ref="E2:E19" si="0">IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
+        <f t="shared" ref="E2:E26" si="0">IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
         <v>7</v>
       </c>
       <c r="F2" s="61">
-        <f t="shared" ref="F2:F19" si="1">IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
+        <f t="shared" ref="F2:F26" si="1">IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
         <v>7</v>
       </c>
       <c r="G2" s="62">
-        <f t="shared" ref="G2:G19" si="2">INDEX(CostPerHour,E2)</f>
+        <f t="shared" ref="G2:G26" si="2">INDEX(CostPerHour,E2)</f>
         <v>591.86</v>
       </c>
       <c r="H2" s="63">
-        <f t="shared" ref="H2:H19" si="3">IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
+        <f t="shared" ref="H2:H26" si="3">IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
         <v>0.5</v>
       </c>
       <c r="I2" s="62">
@@ -2588,7 +2602,7 @@
       </c>
       <c r="J2" s="64"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>75</v>
       </c>
@@ -2623,7 +2637,7 @@
       </c>
       <c r="J3" s="64"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>86</v>
       </c>
@@ -2658,7 +2672,7 @@
       </c>
       <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>93</v>
       </c>
@@ -2695,7 +2709,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>97</v>
       </c>
@@ -2725,14 +2739,14 @@
         <v>1</v>
       </c>
       <c r="I6" s="62">
-        <f t="shared" ref="I6:I19" si="5">D6*G6*H6</f>
+        <f t="shared" ref="I6:I26" si="5">D6*G6*H6</f>
         <v>177.56</v>
       </c>
       <c r="J6" s="64" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>101</v>
       </c>
@@ -2769,7 +2783,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>102</v>
       </c>
@@ -2806,7 +2820,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
         <v>102</v>
       </c>
@@ -2843,7 +2857,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
         <v>103</v>
       </c>
@@ -2880,7 +2894,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
         <v>108</v>
       </c>
@@ -2917,7 +2931,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
         <v>108</v>
       </c>
@@ -2954,7 +2968,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>111</v>
       </c>
@@ -2991,7 +3005,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
         <v>111</v>
       </c>
@@ -3028,7 +3042,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
         <v>115</v>
       </c>
@@ -3065,18 +3079,26 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="58"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="60">
+        <v>2</v>
+      </c>
       <c r="E16" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F16" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="62">
         <f t="shared" si="2"/>
@@ -3084,26 +3106,36 @@
       </c>
       <c r="H16" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="64"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="58"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60"/>
+        <v>236.74</v>
+      </c>
+      <c r="J16" s="64" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="60">
+        <v>3</v>
+      </c>
       <c r="E17" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F17" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="62">
         <f t="shared" si="2"/>
@@ -3111,15 +3143,17 @@
       </c>
       <c r="H17" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="64"/>
-    </row>
-    <row r="18" spans="1:10">
+        <v>532.68000000000006</v>
+      </c>
+      <c r="J17" s="64" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="58"/>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
@@ -3134,7 +3168,7 @@
       </c>
       <c r="G18" s="62">
         <f t="shared" si="2"/>
-        <v>118.37</v>
+        <v>71.02</v>
       </c>
       <c r="H18" s="63">
         <f t="shared" si="3"/>
@@ -3146,7 +3180,7 @@
       </c>
       <c r="J18" s="64"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="58"/>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
@@ -3161,7 +3195,7 @@
       </c>
       <c r="G19" s="62">
         <f t="shared" si="2"/>
-        <v>591.86</v>
+        <v>35.51</v>
       </c>
       <c r="H19" s="63">
         <f t="shared" si="3"/>
@@ -3172,6 +3206,195 @@
         <v>0</v>
       </c>
       <c r="J19" s="64"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="58"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="62">
+        <f t="shared" si="2"/>
+        <v>236.74</v>
+      </c>
+      <c r="H20" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="64"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="58"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="62">
+        <f t="shared" si="2"/>
+        <v>71.02</v>
+      </c>
+      <c r="H21" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="64"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="58"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="62">
+        <f t="shared" si="2"/>
+        <v>35.51</v>
+      </c>
+      <c r="H22" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="64"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="58"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="62">
+        <f t="shared" si="2"/>
+        <v>71.02</v>
+      </c>
+      <c r="H23" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="64"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="58"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="62">
+        <f t="shared" si="2"/>
+        <v>35.51</v>
+      </c>
+      <c r="H24" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="64"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="58"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="62">
+        <f t="shared" si="2"/>
+        <v>71.02</v>
+      </c>
+      <c r="H25" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="64"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="58"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="62">
+        <f t="shared" si="2"/>
+        <v>35.51</v>
+      </c>
+      <c r="H26" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="64"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -3187,14 +3410,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -3209,7 +3432,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -3241,7 +3464,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58"/>
       <c r="B2" s="59" t="s">
         <v>8</v>
@@ -3272,7 +3495,7 @@
       </c>
       <c r="J2" s="64"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58"/>
       <c r="B3" s="59" t="s">
         <v>8</v>
@@ -3303,7 +3526,7 @@
       </c>
       <c r="J3" s="64"/>
     </row>
-    <row r="4" spans="1:10" ht="30">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>75</v>
       </c>
@@ -3340,7 +3563,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>75</v>
       </c>
@@ -3377,7 +3600,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>86</v>
       </c>
@@ -3414,7 +3637,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>86</v>
       </c>
@@ -3451,7 +3674,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="58"/>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -3477,14 +3700,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -3499,7 +3722,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -3531,7 +3754,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>75</v>
       </c>
@@ -3568,7 +3791,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>75</v>
       </c>
@@ -3605,7 +3828,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>75</v>
       </c>
@@ -3642,7 +3865,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -3669,7 +3892,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -3710,14 +3933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -3732,7 +3955,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -3764,7 +3987,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>84</v>
       </c>
@@ -3801,7 +4024,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>99</v>
       </c>
@@ -3838,7 +4061,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -3865,7 +4088,7 @@
       </c>
       <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -3892,7 +4115,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -3933,14 +4156,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -3953,7 +4176,7 @@
     <col min="30" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="91" t="s">
         <v>81</v>
       </c>
@@ -3994,7 +4217,7 @@
       <c r="AH1" s="89"/>
       <c r="AI1" s="90"/>
     </row>
-    <row r="2" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="92"/>
       <c r="B2" s="92"/>
       <c r="C2" s="93" t="s">
@@ -4041,7 +4264,7 @@
       <c r="AH2" s="86"/>
       <c r="AI2" s="87"/>
     </row>
-    <row r="3" spans="1:35" ht="180">
+    <row r="3" spans="1:35" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
@@ -4148,7 +4371,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
         <v>1</v>
       </c>
@@ -4255,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
         <v>2</v>
       </c>
@@ -4362,7 +4585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="23">
         <v>3</v>
       </c>
@@ -4403,7 +4626,7 @@
       <c r="AH6" s="35"/>
       <c r="AI6" s="44"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>4</v>
       </c>
@@ -4444,7 +4667,7 @@
       <c r="AH7" s="35"/>
       <c r="AI7" s="44"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
         <v>5</v>
       </c>
@@ -4485,7 +4708,7 @@
       <c r="AH8" s="35"/>
       <c r="AI8" s="44"/>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
         <v>6</v>
       </c>
@@ -4526,7 +4749,7 @@
       <c r="AH9" s="35"/>
       <c r="AI9" s="44"/>
     </row>
-    <row r="10" spans="1:35" ht="15.75" thickBot="1">
+    <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>7</v>
       </c>
@@ -4649,12 +4872,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -4664,7 +4887,7 @@
     <col min="7" max="7" width="13.140625" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>69</v>
       </c>
@@ -4687,7 +4910,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="99" t="s">
         <v>25</v>
       </c>
@@ -4714,7 +4937,7 @@
       </c>
       <c r="H2" s="73"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="100"/>
       <c r="B3" s="9">
         <v>2</v>
@@ -4739,7 +4962,7 @@
       </c>
       <c r="H3" s="73"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="100"/>
       <c r="B4" s="9">
         <v>3</v>
@@ -4764,7 +4987,7 @@
       </c>
       <c r="H4" s="73"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="100"/>
       <c r="B5" s="9">
         <v>4</v>
@@ -4789,7 +5012,7 @@
       </c>
       <c r="H5" s="73"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="100"/>
       <c r="B6" s="9">
         <v>5</v>
@@ -4814,7 +5037,7 @@
       </c>
       <c r="H6" s="73"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="101"/>
       <c r="B7" s="9">
         <v>6</v>
@@ -4839,7 +5062,7 @@
       </c>
       <c r="H7" s="73"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="99" t="s">
         <v>29</v>
       </c>
@@ -4865,7 +5088,7 @@
         <v>591.86</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="100"/>
       <c r="B9" s="9">
         <v>8</v>
@@ -4889,7 +5112,7 @@
         <v>236.74</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
       <c r="B10" s="9">
         <v>9</v>
@@ -4913,7 +5136,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="100"/>
       <c r="B11" s="9">
         <v>10</v>
@@ -4937,7 +5160,7 @@
         <v>591.86</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="100"/>
       <c r="B12" s="9">
         <v>11</v>
@@ -4961,7 +5184,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="100"/>
       <c r="B13" s="9">
         <v>12</v>
@@ -4985,7 +5208,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="100"/>
       <c r="B14" s="9">
         <v>13</v>
@@ -5009,7 +5232,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="100"/>
       <c r="B15" s="9">
         <v>14</v>
@@ -5033,7 +5256,7 @@
         <v>295.93</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="100"/>
       <c r="B16" s="9">
         <v>15</v>
@@ -5057,7 +5280,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="99" t="s">
         <v>67</v>
       </c>
@@ -5083,7 +5306,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="100"/>
       <c r="B18" s="9">
         <v>17</v>
@@ -5107,7 +5330,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
       <c r="B19" s="9">
         <v>18</v>
@@ -5131,7 +5354,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="100"/>
       <c r="B20" s="9">
         <v>19</v>
@@ -5155,7 +5378,7 @@
         <v>236.74</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="100"/>
       <c r="B21" s="9">
         <v>20</v>
@@ -5179,7 +5402,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="100"/>
       <c r="B22" s="9">
         <v>21</v>
@@ -5203,7 +5426,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="100"/>
       <c r="B23" s="9">
         <v>22</v>
@@ -5227,7 +5450,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="100"/>
       <c r="B24" s="9">
         <v>23</v>
@@ -5251,7 +5474,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="100"/>
       <c r="B25" s="9">
         <v>24</v>
@@ -5275,7 +5498,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="101"/>
       <c r="B26" s="9">
         <v>25</v>
@@ -5299,7 +5522,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="99" t="s">
         <v>68</v>
       </c>
@@ -5325,7 +5548,7 @@
         <v>295.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="100"/>
       <c r="B28" s="9">
         <v>27</v>
@@ -5349,7 +5572,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="100"/>
       <c r="B29" s="9">
         <v>28</v>
@@ -5373,7 +5596,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="101"/>
       <c r="B30" s="9">
         <v>29</v>
@@ -5397,7 +5620,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="99" t="s">
         <v>28</v>
       </c>
@@ -5423,7 +5646,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="100"/>
       <c r="B32" s="9">
         <v>31</v>
@@ -5447,7 +5670,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="100"/>
       <c r="B33" s="9">
         <v>32</v>
@@ -5471,7 +5694,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="100"/>
       <c r="B34" s="9">
         <v>33</v>

</xml_diff>

<commit_message>
Reverting school and adding Brij's effort at end
</commit_message>
<xml_diff>
--- a/Project Management/Effort Calculation.xlsx
+++ b/Project Management/Effort Calculation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="330" windowWidth="18795" windowHeight="11700" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="8" r:id="rId1"/>
@@ -24,12 +24,12 @@
     <definedName name="MemberList">'Team Member'!$B$4:$B$10</definedName>
     <definedName name="SkillList">'Skill Set'!$C$2:$C$34</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="123">
   <si>
     <t>Total</t>
   </si>
@@ -379,26 +379,35 @@
     <t>06.11.2015</t>
   </si>
   <si>
+    <t>07.11.2015</t>
+  </si>
+  <si>
+    <t>Wireframe for student</t>
+  </si>
+  <si>
     <t>10.11.2015</t>
   </si>
   <si>
+    <t>Billing design, discussion for fees</t>
+  </si>
+  <si>
     <t>System Setup and Project Understanding</t>
   </si>
   <si>
+    <t>Developed component for Caste,Class,Category,Section,Landline,Mobile, Subcaste</t>
+  </si>
+  <si>
     <t>11.11.2015</t>
-  </si>
-  <si>
-    <t>Developed component for Caste,Class,Category,Section,Landline,Mobile, Subcaste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1210,6 +1219,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1244,6 +1254,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1419,12 +1430,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="1"/>
@@ -1432,8 +1443,8 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:15">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -1449,7 +1460,7 @@
       <c r="N2" s="19"/>
       <c r="O2" s="20"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1465,7 +1476,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="21"/>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1481,7 +1492,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="21"/>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1497,7 +1508,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="21"/>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1513,7 +1524,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="21"/>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1529,7 +1540,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="21"/>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1545,7 +1556,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="21"/>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1561,7 +1572,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="21"/>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1579,7 +1590,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="21"/>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1590,7 +1601,7 @@
       <c r="G11" s="77"/>
       <c r="H11" s="81">
         <f>Summery!D10</f>
-        <v>16512.806500000002</v>
+        <v>17282.226500000001</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="83"/>
@@ -1600,7 +1611,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="21"/>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1611,7 +1622,7 @@
       <c r="G12" s="77"/>
       <c r="H12" s="78">
         <f>Summery!C10</f>
-        <v>64.5</v>
+        <v>69.5</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="80"/>
@@ -1621,7 +1632,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="21"/>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1632,7 +1643,7 @@
       <c r="G13" s="77"/>
       <c r="H13" s="78">
         <f>H12/8</f>
-        <v>8.0625</v>
+        <v>8.6875</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="80"/>
@@ -1642,7 +1653,7 @@
       <c r="N13" s="4"/>
       <c r="O13" s="21"/>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1658,7 +1669,7 @@
       <c r="N14" s="4"/>
       <c r="O14" s="21"/>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1674,7 +1685,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1690,7 +1701,7 @@
       <c r="N16" s="4"/>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
@@ -1705,7 +1716,7 @@
       <c r="N17" s="4"/>
       <c r="O17" s="21"/>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1720,7 +1731,7 @@
       <c r="N18" s="4"/>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1736,7 +1747,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="2:15" ht="15.75" thickBot="1">
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1769,14 +1780,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
@@ -1798,7 +1809,7 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="84" t="s">
         <v>61</v>
@@ -1821,7 +1832,7 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="11" t="s">
         <v>6</v>
@@ -1852,18 +1863,18 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="14">
         <f>SUMIF(Business!B:B,B3,Business!D:D) + SUMIF(School!B:B,B3,School!D:D) + SUMIF(Service!B:B,B3,Service!D:D)+SUMIF(Retail!B:B,B3,Retail!D:D) + SUMIF(Tourism!B:B,B3,Tourism!D:D)</f>
-        <v>39.5</v>
+        <v>44.5</v>
       </c>
       <c r="D3" s="33">
         <f>SUMIF(Business!B:B,B3,Business!I:I) + SUMIF(School!B:B,B3,School!I:I) + SUMIF(Service!B:B,B3,Service!I:I)+SUMIF(Retail!B:B,B3,Retail!I:I) + SUMIF(Tourism!B:B,B3,Tourism!I:I)</f>
-        <v>12458.585000000001</v>
+        <v>13228.005000000001</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
@@ -1887,7 +1898,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="10" t="s">
         <v>10</v>
@@ -1906,11 +1917,11 @@
       </c>
       <c r="G4" s="14">
         <f>SUM(School!D:D)</f>
-        <v>40.5</v>
+        <v>45.5</v>
       </c>
       <c r="H4" s="33">
         <f>SUM(School!I:I)</f>
-        <v>6747.1574999999975</v>
+        <v>7516.5774999999976</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -1922,7 +1933,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
@@ -1957,7 +1968,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="10" t="s">
         <v>11</v>
@@ -1992,7 +2003,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="10" t="s">
         <v>12</v>
@@ -2027,7 +2038,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="10" t="s">
         <v>13</v>
@@ -2046,11 +2057,11 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G3:G7)</f>
-        <v>64.5</v>
+        <v>69.5</v>
       </c>
       <c r="H8" s="34">
         <f>SUM(H3:H7)</f>
-        <v>16512.806499999995</v>
+        <v>17282.226499999997</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -2062,7 +2073,7 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="10" t="s">
         <v>14</v>
@@ -2089,18 +2100,18 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="15">
         <f>SUM(C3:C9)</f>
-        <v>64.5</v>
+        <v>69.5</v>
       </c>
       <c r="D10" s="34">
         <f>SUM(D3:D9)</f>
-        <v>16512.806500000002</v>
+        <v>17282.226500000001</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -2116,7 +2127,7 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="16"/>
@@ -2132,7 +2143,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="16"/>
@@ -2148,7 +2159,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="16"/>
@@ -2167,7 +2178,7 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="16"/>
@@ -2186,7 +2197,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="16"/>
@@ -2205,7 +2216,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="16"/>
@@ -2224,7 +2235,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="16"/>
@@ -2243,7 +2254,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="16"/>
@@ -2277,14 +2288,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -2299,7 +2310,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>4</v>
       </c>
@@ -2331,7 +2342,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>51</v>
       </c>
@@ -2368,7 +2379,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>88</v>
       </c>
@@ -2405,7 +2416,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>93</v>
       </c>
@@ -2442,7 +2453,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -2469,7 +2480,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -2511,14 +2522,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -2533,7 +2544,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -2565,7 +2576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>95</v>
       </c>
@@ -2579,19 +2590,19 @@
         <v>2</v>
       </c>
       <c r="E2" s="61">
-        <f t="shared" ref="E2:E19" si="0">IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
+        <f t="shared" ref="E2:E26" si="0">IF(ISERROR(MATCH(C2,SkillList,0)),0,MATCH(C2,SkillList,0))</f>
         <v>7</v>
       </c>
       <c r="F2" s="61">
-        <f t="shared" ref="F2:F19" si="1">IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
+        <f t="shared" ref="F2:F26" si="1">IF(ISERROR(MATCH(B2,MemberList,0)),0,MATCH(B2,MemberList,0))</f>
         <v>7</v>
       </c>
       <c r="G2" s="62">
-        <f t="shared" ref="G2:G19" si="2">INDEX(CostPerHour,E2)</f>
+        <f t="shared" ref="G2:G26" si="2">INDEX(CostPerHour,E2)</f>
         <v>591.86</v>
       </c>
       <c r="H2" s="63">
-        <f t="shared" ref="H2:H19" si="3">IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
+        <f t="shared" ref="H2:H26" si="3">IF(ISERROR(INDEX(Competency,F2,E2)), 0, INDEX(Competency,F2,E2))</f>
         <v>0.5</v>
       </c>
       <c r="I2" s="62">
@@ -2600,7 +2611,7 @@
       </c>
       <c r="J2" s="64"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>75</v>
       </c>
@@ -2635,7 +2646,7 @@
       </c>
       <c r="J3" s="64"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>86</v>
       </c>
@@ -2670,7 +2681,7 @@
       </c>
       <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>93</v>
       </c>
@@ -2707,7 +2718,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>97</v>
       </c>
@@ -2737,14 +2748,14 @@
         <v>1</v>
       </c>
       <c r="I6" s="62">
-        <f t="shared" ref="I6:I19" si="5">D6*G6*H6</f>
+        <f t="shared" ref="I6:I26" si="5">D6*G6*H6</f>
         <v>177.56</v>
       </c>
       <c r="J6" s="64" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>101</v>
       </c>
@@ -2781,7 +2792,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>102</v>
       </c>
@@ -2818,7 +2829,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
         <v>102</v>
       </c>
@@ -2855,7 +2866,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
         <v>103</v>
       </c>
@@ -2892,7 +2903,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
         <v>108</v>
       </c>
@@ -2929,7 +2940,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
         <v>108</v>
       </c>
@@ -2966,7 +2977,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>111</v>
       </c>
@@ -3003,7 +3014,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
         <v>111</v>
       </c>
@@ -3040,7 +3051,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
         <v>115</v>
       </c>
@@ -3077,18 +3088,18 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
         <v>116</v>
       </c>
       <c r="B16" s="59" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C16" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16" s="61">
         <f t="shared" si="0"/>
@@ -3096,7 +3107,7 @@
       </c>
       <c r="F16" s="61">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" s="62">
         <f t="shared" si="2"/>
@@ -3108,36 +3119,36 @@
       </c>
       <c r="I16" s="62">
         <f t="shared" si="5"/>
-        <v>473.48</v>
+        <v>236.74</v>
       </c>
       <c r="J16" s="64" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
         <v>118</v>
       </c>
       <c r="B17" s="59" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C17" s="59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="60">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17" s="61">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="61">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="62">
         <f t="shared" si="2"/>
-        <v>118.37</v>
+        <v>177.56</v>
       </c>
       <c r="H17" s="63">
         <f t="shared" si="3"/>
@@ -3145,65 +3156,274 @@
       </c>
       <c r="I17" s="62">
         <f t="shared" si="5"/>
-        <v>473.48</v>
+        <v>532.68000000000006</v>
       </c>
       <c r="J17" s="64" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="60"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="60">
+        <v>4</v>
+      </c>
       <c r="E18" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F18" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" s="62">
         <f t="shared" si="2"/>
-        <v>71.02</v>
+        <v>118.37</v>
       </c>
       <c r="H18" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="64"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="58"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60"/>
+        <v>473.48</v>
+      </c>
+      <c r="J18" s="64" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="60">
+        <v>4</v>
+      </c>
       <c r="E19" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F19" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19" s="62">
         <f t="shared" si="2"/>
-        <v>35.51</v>
+        <v>118.37</v>
       </c>
       <c r="H19" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="64"/>
+        <v>473.48</v>
+      </c>
+      <c r="J19" s="64" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="58"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="62">
+        <f t="shared" si="2"/>
+        <v>236.74</v>
+      </c>
+      <c r="H20" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="64"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="58"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="62">
+        <f t="shared" si="2"/>
+        <v>71.02</v>
+      </c>
+      <c r="H21" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="64"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="58"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="62">
+        <f t="shared" si="2"/>
+        <v>35.51</v>
+      </c>
+      <c r="H22" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="64"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="58"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="62">
+        <f t="shared" si="2"/>
+        <v>71.02</v>
+      </c>
+      <c r="H23" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="64"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="58"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="62">
+        <f t="shared" si="2"/>
+        <v>35.51</v>
+      </c>
+      <c r="H24" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="64"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="58"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="62">
+        <f t="shared" si="2"/>
+        <v>71.02</v>
+      </c>
+      <c r="H25" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="64"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="58"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="62">
+        <f t="shared" si="2"/>
+        <v>35.51</v>
+      </c>
+      <c r="H26" s="63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="64"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -3219,14 +3439,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -3241,7 +3461,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -3273,7 +3493,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58"/>
       <c r="B2" s="59" t="s">
         <v>8</v>
@@ -3304,7 +3524,7 @@
       </c>
       <c r="J2" s="64"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58"/>
       <c r="B3" s="59" t="s">
         <v>8</v>
@@ -3335,7 +3555,7 @@
       </c>
       <c r="J3" s="64"/>
     </row>
-    <row r="4" spans="1:10" ht="30">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>75</v>
       </c>
@@ -3372,7 +3592,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>75</v>
       </c>
@@ -3409,7 +3629,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>86</v>
       </c>
@@ -3446,7 +3666,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>86</v>
       </c>
@@ -3483,7 +3703,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="58"/>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -3509,14 +3729,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -3531,7 +3751,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -3563,7 +3783,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>75</v>
       </c>
@@ -3600,7 +3820,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>75</v>
       </c>
@@ -3637,7 +3857,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>75</v>
       </c>
@@ -3674,7 +3894,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -3701,7 +3921,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -3742,14 +3962,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="57" bestFit="1" customWidth="1"/>
@@ -3764,7 +3984,7 @@
     <col min="11" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
@@ -3796,7 +4016,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>84</v>
       </c>
@@ -3833,7 +4053,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>99</v>
       </c>
@@ -3870,7 +4090,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="58"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -3897,7 +4117,7 @@
       </c>
       <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -3924,7 +4144,7 @@
       </c>
       <c r="J5" s="64"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -3965,14 +4185,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -3985,7 +4205,7 @@
     <col min="30" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="91" t="s">
         <v>81</v>
       </c>
@@ -4026,7 +4246,7 @@
       <c r="AH1" s="89"/>
       <c r="AI1" s="90"/>
     </row>
-    <row r="2" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="92"/>
       <c r="B2" s="92"/>
       <c r="C2" s="93" t="s">
@@ -4073,7 +4293,7 @@
       <c r="AH2" s="86"/>
       <c r="AI2" s="87"/>
     </row>
-    <row r="3" spans="1:35" ht="180">
+    <row r="3" spans="1:35" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
@@ -4180,7 +4400,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
         <v>1</v>
       </c>
@@ -4287,7 +4507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
         <v>2</v>
       </c>
@@ -4394,7 +4614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="23">
         <v>3</v>
       </c>
@@ -4435,7 +4655,7 @@
       <c r="AH6" s="35"/>
       <c r="AI6" s="44"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>4</v>
       </c>
@@ -4476,7 +4696,7 @@
       <c r="AH7" s="35"/>
       <c r="AI7" s="44"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
         <v>5</v>
       </c>
@@ -4517,7 +4737,7 @@
       <c r="AH8" s="35"/>
       <c r="AI8" s="44"/>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
         <v>6</v>
       </c>
@@ -4558,7 +4778,7 @@
       <c r="AH9" s="35"/>
       <c r="AI9" s="44"/>
     </row>
-    <row r="10" spans="1:35" ht="15.75" thickBot="1">
+    <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>7</v>
       </c>
@@ -4681,12 +4901,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -4696,7 +4916,7 @@
     <col min="7" max="7" width="13.140625" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>69</v>
       </c>
@@ -4719,7 +4939,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="99" t="s">
         <v>25</v>
       </c>
@@ -4746,7 +4966,7 @@
       </c>
       <c r="H2" s="73"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="100"/>
       <c r="B3" s="9">
         <v>2</v>
@@ -4771,7 +4991,7 @@
       </c>
       <c r="H3" s="73"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="100"/>
       <c r="B4" s="9">
         <v>3</v>
@@ -4796,7 +5016,7 @@
       </c>
       <c r="H4" s="73"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="100"/>
       <c r="B5" s="9">
         <v>4</v>
@@ -4821,7 +5041,7 @@
       </c>
       <c r="H5" s="73"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="100"/>
       <c r="B6" s="9">
         <v>5</v>
@@ -4846,7 +5066,7 @@
       </c>
       <c r="H6" s="73"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="101"/>
       <c r="B7" s="9">
         <v>6</v>
@@ -4871,7 +5091,7 @@
       </c>
       <c r="H7" s="73"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="99" t="s">
         <v>29</v>
       </c>
@@ -4897,7 +5117,7 @@
         <v>591.86</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="100"/>
       <c r="B9" s="9">
         <v>8</v>
@@ -4921,7 +5141,7 @@
         <v>236.74</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
       <c r="B10" s="9">
         <v>9</v>
@@ -4945,7 +5165,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="100"/>
       <c r="B11" s="9">
         <v>10</v>
@@ -4969,7 +5189,7 @@
         <v>591.86</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="100"/>
       <c r="B12" s="9">
         <v>11</v>
@@ -4993,7 +5213,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="100"/>
       <c r="B13" s="9">
         <v>12</v>
@@ -5017,7 +5237,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="100"/>
       <c r="B14" s="9">
         <v>13</v>
@@ -5041,7 +5261,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="100"/>
       <c r="B15" s="9">
         <v>14</v>
@@ -5065,7 +5285,7 @@
         <v>295.93</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="100"/>
       <c r="B16" s="9">
         <v>15</v>
@@ -5089,7 +5309,7 @@
         <v>118.37</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="99" t="s">
         <v>67</v>
       </c>
@@ -5115,7 +5335,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="100"/>
       <c r="B18" s="9">
         <v>17</v>
@@ -5139,7 +5359,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
       <c r="B19" s="9">
         <v>18</v>
@@ -5163,7 +5383,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="100"/>
       <c r="B20" s="9">
         <v>19</v>
@@ -5187,7 +5407,7 @@
         <v>236.74</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="100"/>
       <c r="B21" s="9">
         <v>20</v>
@@ -5211,7 +5431,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="100"/>
       <c r="B22" s="9">
         <v>21</v>
@@ -5235,7 +5455,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="100"/>
       <c r="B23" s="9">
         <v>22</v>
@@ -5259,7 +5479,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="100"/>
       <c r="B24" s="9">
         <v>23</v>
@@ -5283,7 +5503,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="100"/>
       <c r="B25" s="9">
         <v>24</v>
@@ -5307,7 +5527,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="101"/>
       <c r="B26" s="9">
         <v>25</v>
@@ -5331,7 +5551,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="99" t="s">
         <v>68</v>
       </c>
@@ -5357,7 +5577,7 @@
         <v>295.93</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="100"/>
       <c r="B28" s="9">
         <v>27</v>
@@ -5381,7 +5601,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="100"/>
       <c r="B29" s="9">
         <v>28</v>
@@ -5405,7 +5625,7 @@
         <v>177.56</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="101"/>
       <c r="B30" s="9">
         <v>29</v>
@@ -5429,7 +5649,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="99" t="s">
         <v>28</v>
       </c>
@@ -5455,7 +5675,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="100"/>
       <c r="B32" s="9">
         <v>31</v>
@@ -5479,7 +5699,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="100"/>
       <c r="B33" s="9">
         <v>32</v>
@@ -5503,7 +5723,7 @@
         <v>71.02</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="100"/>
       <c r="B34" s="9">
         <v>33</v>

</xml_diff>